<commit_message>
Take a copy of colours
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6DFE4F-A45A-C94E-BF92-D0D9B414FB85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F72125-517C-9A4A-8EB0-590BF9FB4B6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="2140" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="110">
   <si>
     <t>Storyboard</t>
   </si>
@@ -349,10 +349,19 @@
     <t>Error score cells</t>
   </si>
   <si>
-    <t>Thumbnail initials, menu background</t>
-  </si>
-  <si>
     <t>Menu title</t>
+  </si>
+  <si>
+    <t>Thumbnail disc</t>
+  </si>
+  <si>
+    <t>Thumbnail disc for initials</t>
+  </si>
+  <si>
+    <t>Popup menus background</t>
+  </si>
+  <si>
+    <t>Popup menus title</t>
   </si>
 </sst>
 </file>
@@ -425,7 +434,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +552,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3C30"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1E5C9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -645,6 +660,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -656,6 +674,7 @@
   <colors>
     <mruColors>
       <color rgb="FF7F7F7F"/>
+      <color rgb="FFF1E5C9"/>
       <color rgb="FFFF3C30"/>
       <color rgb="FF27CD41"/>
       <color rgb="FFFF3B30"/>
@@ -664,7 +683,6 @@
       <color rgb="FFFFFFFF"/>
       <color rgb="FFE6BF5F"/>
       <color rgb="FF7F7F80"/>
-      <color rgb="FFEB3021"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1157,13 +1175,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
-  <dimension ref="A1:AH27"/>
+  <dimension ref="A1:AH28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,6 +1322,9 @@
       <c r="K2" t="s">
         <v>103</v>
       </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1349,6 +1370,9 @@
       <c r="E5" t="s">
         <v>64</v>
       </c>
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
       <c r="H5" t="s">
         <v>80</v>
       </c>
@@ -1367,7 +1391,7 @@
         <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H6" t="s">
         <v>81</v>
@@ -1412,7 +1436,7 @@
         <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H9" t="s">
         <v>82</v>
@@ -1487,97 +1511,96 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" t="s">
-        <v>75</v>
+        <v>106</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J18" t="s">
-        <v>89</v>
+        <v>78</v>
+      </c>
+      <c r="H18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="K19" t="s">
-        <v>92</v>
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="25"/>
+        <v>49</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="E20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" t="s">
-        <v>101</v>
+        <v>56</v>
+      </c>
+      <c r="K20" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="26"/>
+        <v>93</v>
+      </c>
+      <c r="B21" s="25"/>
       <c r="E21" t="s">
         <v>99</v>
       </c>
@@ -1587,9 +1610,9 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="27"/>
+        <v>94</v>
+      </c>
+      <c r="B22" s="26"/>
       <c r="E22" t="s">
         <v>99</v>
       </c>
@@ -1599,21 +1622,21 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="28"/>
+        <v>98</v>
+      </c>
+      <c r="B23" s="27"/>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="29"/>
+        <v>96</v>
+      </c>
+      <c r="B24" s="28"/>
       <c r="E24" t="s">
         <v>100</v>
       </c>
@@ -1623,9 +1646,9 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="27"/>
+        <v>97</v>
+      </c>
+      <c r="B25" s="29"/>
       <c r="E25" t="s">
         <v>100</v>
       </c>
@@ -1635,33 +1658,45 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="14"/>
+        <v>95</v>
+      </c>
+      <c r="B26" s="27"/>
       <c r="E26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" t="s">
-        <v>73</v>
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="14"/>
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="13"/>
-      <c r="E27" t="s">
+      <c r="B28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="13"/>
+      <c r="E28" t="s">
         <v>59</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nearly complete version of palette implemented - changed sync model
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F72125-517C-9A4A-8EB0-590BF9FB4B6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7FA7CF-23DA-C742-A6EC-16BDF52A6F2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="2140" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="2180" yWindow="1040" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Storyboards" sheetId="1" r:id="rId1"/>
     <sheet name="Colors" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="210">
   <si>
     <t>Storyboard</t>
   </si>
@@ -157,18 +157,12 @@
     <t>Made Contract</t>
   </si>
   <si>
-    <t>Message</t>
-  </si>
-  <si>
     <t>Section Heading</t>
   </si>
   <si>
     <t>Shape Fill</t>
   </si>
   <si>
-    <t>Shape Highlight</t>
-  </si>
-  <si>
     <t>Table Top</t>
   </si>
   <si>
@@ -184,12 +178,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Stroke</t>
-  </si>
-  <si>
-    <t>Fill</t>
-  </si>
-  <si>
     <t>Default background color for views</t>
   </si>
   <si>
@@ -244,9 +232,6 @@
     <t>Background for made contracts in scorecard</t>
   </si>
   <si>
-    <t>Messages</t>
-  </si>
-  <si>
     <t>Banner / Logo</t>
   </si>
   <si>
@@ -271,9 +256,6 @@
     <t>Network/iCloud message</t>
   </si>
   <si>
-    <t>Outline of email box</t>
-  </si>
-  <si>
     <t>Home Screen button</t>
   </si>
   <si>
@@ -362,13 +344,361 @@
   </si>
   <si>
     <t>Popup menus title</t>
+  </si>
+  <si>
+    <t>Banner &amp; status bar</t>
+  </si>
+  <si>
+    <t>Player names</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Bid / score buttons / cursor</t>
+  </si>
+  <si>
+    <t>Done button</t>
+  </si>
+  <si>
+    <t>Banner, title &amp; status bar</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Round summary icon and undo arrow are dark highlight color</t>
+  </si>
+  <si>
+    <t>Text Inverse</t>
+  </si>
+  <si>
+    <t>Background / Text</t>
+  </si>
+  <si>
+    <t>Shape Stroke</t>
+  </si>
+  <si>
+    <t>Shape Highlight Fill</t>
+  </si>
+  <si>
+    <t>Shape Highlight Stroke</t>
+  </si>
+  <si>
+    <t>Background of thumbnail when showing initials</t>
+  </si>
+  <si>
+    <t>Separator</t>
+  </si>
+  <si>
+    <t>Separator color in tables</t>
+  </si>
+  <si>
+    <t>Separtors between names</t>
+  </si>
+  <si>
+    <t>Dealer Button</t>
+  </si>
+  <si>
+    <t>Grid</t>
+  </si>
+  <si>
+    <t>Scorepad grid</t>
+  </si>
+  <si>
+    <t>Dealer</t>
+  </si>
+  <si>
+    <t>Error done/info button</t>
+  </si>
+  <si>
+    <t>Separator between names</t>
+  </si>
+  <si>
+    <t>Main background/bids</t>
+  </si>
+  <si>
+    <t>Trump suit</t>
+  </si>
+  <si>
+    <t>Contract over/under</t>
+  </si>
+  <si>
+    <t>Main background/scores</t>
+  </si>
+  <si>
+    <t>Buttons assume a dark background</t>
+  </si>
+  <si>
+    <t>Banner / search input</t>
+  </si>
+  <si>
+    <t>Background of search matches</t>
+  </si>
+  <si>
+    <t>Search matches</t>
+  </si>
+  <si>
+    <t>Card Face</t>
+  </si>
+  <si>
+    <t>Card Back</t>
+  </si>
+  <si>
+    <t>Card face &amp; back outline</t>
+  </si>
+  <si>
+    <t>Card back</t>
+  </si>
+  <si>
+    <t>Card back outline</t>
+  </si>
+  <si>
+    <t>Background / players / outcome</t>
+  </si>
+  <si>
+    <t>Select Players</t>
+  </si>
+  <si>
+    <t>Bidding background</t>
+  </si>
+  <si>
+    <t>Card faces</t>
+  </si>
+  <si>
+    <t>Hand area</t>
+  </si>
+  <si>
+    <t>Table top for cards</t>
+  </si>
+  <si>
+    <t>Bidding buttons</t>
+  </si>
+  <si>
+    <t>Seaparators in bid view</t>
+  </si>
+  <si>
+    <t>Text for player names</t>
+  </si>
+  <si>
+    <t>Banner when your turn</t>
+  </si>
+  <si>
+    <t>Banner when not your turn</t>
+  </si>
+  <si>
+    <t>Disabled bid buttons use same color with 30% alpha</t>
+  </si>
+  <si>
+    <t>Contract button in banner</t>
+  </si>
+  <si>
+    <t>Card values</t>
+  </si>
+  <si>
+    <t>Confirm card / bid background</t>
+  </si>
+  <si>
+    <t>Info text &amp; change button</t>
+  </si>
+  <si>
+    <t>Separate modes / players</t>
+  </si>
+  <si>
+    <t>Separate players</t>
+  </si>
+  <si>
+    <t>Use an alpha of 0.3 for services / change button when not available</t>
+  </si>
+  <si>
+    <t>Search bar / instructions / selected</t>
+  </si>
+  <si>
+    <t>Disable option message</t>
+  </si>
+  <si>
+    <t>Background / Banner</t>
+  </si>
+  <si>
+    <t>Square in middle</t>
+  </si>
+  <si>
+    <t>Player names / Actions</t>
+  </si>
+  <si>
+    <t>Player / action detail</t>
+  </si>
+  <si>
+    <t>Section headings</t>
+  </si>
+  <si>
+    <t>Inverse text color</t>
+  </si>
+  <si>
+    <t>Grid borders</t>
+  </si>
+  <si>
+    <t>Card face</t>
+  </si>
+  <si>
+    <t>Banner &amp; insets</t>
+  </si>
+  <si>
+    <t>Players with no photo</t>
+  </si>
+  <si>
+    <t>Player name hard-coded to white on a grey scale gradient overlay</t>
+  </si>
+  <si>
+    <t>Between players</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Headings / sort arrow</t>
+  </si>
+  <si>
+    <t>Background / sort arrow</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Between games</t>
+  </si>
+  <si>
+    <t>Between sections</t>
+  </si>
+  <si>
+    <t>Data titles</t>
+  </si>
+  <si>
+    <t>Data errors</t>
+  </si>
+  <si>
+    <t>Banner / Triangles</t>
+  </si>
+  <si>
+    <t>Location text</t>
+  </si>
+  <si>
+    <t>Update button</t>
+  </si>
+  <si>
+    <t>Player data</t>
+  </si>
+  <si>
+    <t>Players not on device shown in text with 30% alpha</t>
+  </si>
+  <si>
+    <t>Players heading / not included</t>
+  </si>
+  <si>
+    <t>Everything!</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Background in download</t>
+  </si>
+  <si>
+    <t>Titles are shown with 40% alpha in download mode</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Text </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Contrast</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Text </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Contrast</t>
+    </r>
+  </si>
+  <si>
+    <t>Input Control</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Text </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFE6BF5F"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Placeholder</t>
+    </r>
+  </si>
+  <si>
+    <t>Segmented controls/slider</t>
+  </si>
+  <si>
+    <t>Facetime address / cards</t>
+  </si>
+  <si>
+    <t>Suits sequence</t>
+  </si>
+  <si>
+    <t>Change for online player</t>
+  </si>
+  <si>
+    <t>Title message</t>
+  </si>
+  <si>
+    <t>Images are horrible</t>
+  </si>
+  <si>
+    <t>Update messages</t>
+  </si>
+  <si>
+    <t>Banner &amp; Buttons</t>
+  </si>
+  <si>
+    <t>Number to confirm</t>
+  </si>
+  <si>
+    <t>Message and +/-</t>
+  </si>
+  <si>
+    <t>Main form background</t>
+  </si>
+  <si>
+    <t>Message &amp; text</t>
+  </si>
+  <si>
+    <t>Segmented &amp; Sliders</t>
+  </si>
+  <si>
+    <t>Between buttons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -433,8 +763,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFF1EEF0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF999999"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFE6BF5F"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,12 +850,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF037AFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7B7B7B"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -516,12 +869,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCE736F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF01A100"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,6 +908,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB9B9B9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0226B3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E5E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -583,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -601,12 +972,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,19 +979,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -647,6 +999,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,14 +1014,60 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,16 +1077,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF7F7F7F"/>
-      <color rgb="FFF1E5C9"/>
-      <color rgb="FFFF3C30"/>
-      <color rgb="FF27CD41"/>
-      <color rgb="FFFF3B30"/>
-      <color rgb="FF047AFF"/>
-      <color rgb="FFF1EFEE"/>
-      <color rgb="FFFFFFFF"/>
       <color rgb="FFE6BF5F"/>
       <color rgb="FF7F7F80"/>
+      <color rgb="FFF1E5C9"/>
+      <color rgb="FF999999"/>
+      <color rgb="FFBFBFBF"/>
+      <color rgb="FF80807E"/>
+      <color rgb="FFE7E5E8"/>
+      <color rgb="FF0226B3"/>
+      <color rgb="FFB9B9B9"/>
+      <color rgb="FFF1EEF0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1002,12 +1406,12 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2:A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,142 +1431,142 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1175,529 +1579,1005 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
-  <dimension ref="A1:AH28"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="38.5" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="34" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="33" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="31" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="I1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="J1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="K1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="L1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="M1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="N1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="O1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="P1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="Q1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="R1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="S1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" s="22" t="s">
+      <c r="T1" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="22" t="s">
+      <c r="V1" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="22" t="s">
+      <c r="Y1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="22" t="s">
+      <c r="Z1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="22" t="s">
+      <c r="AA1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="22" t="s">
+      <c r="AB1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="22" t="s">
+      <c r="AC1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="22" t="s">
+      <c r="AD1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="22" t="s">
+      <c r="AE1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="22" t="s">
+      <c r="AF1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="22" t="s">
+      <c r="AG1" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>133</v>
+      </c>
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>142</v>
+      </c>
+      <c r="T2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" t="s">
+        <v>175</v>
+      </c>
+      <c r="W2" t="s">
+        <v>175</v>
+      </c>
+      <c r="X2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
         <v>34</v>
       </c>
       <c r="J3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M3" t="s">
+        <v>132</v>
+      </c>
+      <c r="O3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>150</v>
+      </c>
+      <c r="T3" t="s">
+        <v>104</v>
+      </c>
+      <c r="U3" t="s">
+        <v>169</v>
+      </c>
+      <c r="V3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" s="36" customFormat="1" ht="34">
+      <c r="A5" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="N5" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="R5" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="S5" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y5" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" s="36" customFormat="1" ht="17">
+      <c r="A6" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA6"/>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="I8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" t="s">
         <v>64</v>
       </c>
-      <c r="F5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>159</v>
+      </c>
+      <c r="R10" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
         <v>65</v>
       </c>
-      <c r="F6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" t="s">
-        <v>90</v>
-      </c>
-      <c r="K9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" t="s">
+        <v>165</v>
+      </c>
+      <c r="P13" t="s">
+        <v>165</v>
+      </c>
+      <c r="T13" t="s">
+        <v>165</v>
+      </c>
+      <c r="V13" t="s">
+        <v>174</v>
+      </c>
+      <c r="W13" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="R15" t="s">
+        <v>145</v>
+      </c>
+      <c r="S15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="U16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" s="27" customFormat="1">
+      <c r="A20" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="E20" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" s="27" customFormat="1">
+      <c r="A21" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" t="s">
+        <v>105</v>
+      </c>
+      <c r="M22" t="s">
+        <v>134</v>
+      </c>
+      <c r="R22" t="s">
+        <v>148</v>
+      </c>
+      <c r="T22" t="s">
+        <v>163</v>
+      </c>
+      <c r="V22" t="s">
+        <v>173</v>
+      </c>
+      <c r="W22" t="s">
+        <v>173</v>
+      </c>
+      <c r="X22" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" t="s">
+        <v>98</v>
+      </c>
+      <c r="X25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="O26" t="s">
+        <v>155</v>
+      </c>
+      <c r="P26" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>160</v>
+      </c>
+      <c r="T26" t="s">
+        <v>164</v>
+      </c>
+      <c r="X26" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
+      <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" t="s">
+        <v>120</v>
+      </c>
+      <c r="J28" t="s">
+        <v>126</v>
+      </c>
+      <c r="O28" t="s">
+        <v>156</v>
+      </c>
+      <c r="P28" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>157</v>
+      </c>
+      <c r="R28" t="s">
+        <v>147</v>
+      </c>
+      <c r="V28" t="s">
+        <v>172</v>
+      </c>
+      <c r="W28" t="s">
+        <v>178</v>
+      </c>
+      <c r="X28" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
+      <c r="A29" t="s">
         <v>87</v>
       </c>
-      <c r="J19" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" t="s">
+        <v>95</v>
+      </c>
+      <c r="K29" t="s">
+        <v>128</v>
+      </c>
+      <c r="N29" t="s">
+        <v>153</v>
+      </c>
+      <c r="R29" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
+        <v>95</v>
+      </c>
+      <c r="K30" t="s">
+        <v>128</v>
+      </c>
+      <c r="N30" t="s">
+        <v>153</v>
+      </c>
+      <c r="R30" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>95</v>
+      </c>
+      <c r="K31" t="s">
+        <v>128</v>
+      </c>
+      <c r="N31" t="s">
+        <v>153</v>
+      </c>
+      <c r="R31" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
+      <c r="A32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" t="s">
+        <v>168</v>
+      </c>
+      <c r="D32" t="s">
+        <v>137</v>
+      </c>
+      <c r="N32" t="s">
+        <v>139</v>
+      </c>
+      <c r="R32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29">
+      <c r="A33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" t="s">
+        <v>138</v>
+      </c>
+      <c r="N33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" t="s">
+        <v>96</v>
+      </c>
+      <c r="K34" t="s">
+        <v>129</v>
+      </c>
+      <c r="R34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>96</v>
+      </c>
+      <c r="K35" t="s">
+        <v>129</v>
+      </c>
+      <c r="R35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
+      <c r="A36" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="E21" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="E22" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="E23" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D36" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="E24" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="29"/>
-      <c r="E25" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="E26" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="14"/>
-      <c r="E27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="13"/>
-      <c r="E28" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28" t="s">
-        <v>72</v>
+      <c r="K36" t="s">
+        <v>129</v>
+      </c>
+      <c r="R36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" s="22" customFormat="1" ht="51">
+      <c r="A37" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="J37" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="L37" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="P37" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="R37" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="U37" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="X37" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y37" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC37" s="22" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes after initial feedback from Jack
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1720DC76-99E4-AE49-813D-DD447BCC7527}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E333F3-D0BB-2A47-BF97-DE43BFD93748}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="1040" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -796,7 +796,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -836,12 +836,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEB3021"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF418E92"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,6 +929,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FE3AB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5AA8AB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -957,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -978,10 +984,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1002,6 +1005,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1014,10 +1020,7 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1029,32 +1032,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1063,14 +1066,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1080,6 +1089,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF5AA8AB"/>
+      <color rgb="FF9FE3AB"/>
+      <color rgb="FFACFAD6"/>
       <color rgb="FFE6BF5F"/>
       <color rgb="FF7F7F80"/>
       <color rgb="FFF1E5C9"/>
@@ -1087,9 +1099,6 @@
       <color rgb="FFBFBFBF"/>
       <color rgb="FF80807E"/>
       <color rgb="FFE7E5E8"/>
-      <color rgb="FF0226B3"/>
-      <color rgb="FFB9B9B9"/>
-      <color rgb="FFF1EEF0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1585,10 +1594,10 @@
   <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Z4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE37" sqref="AE37"/>
+      <selection pane="bottomRight" activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1613,91 +1622,91 @@
       <c r="D1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="X1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AA1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AB1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AC1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AD1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AE1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="13" t="s">
+      <c r="AF1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AG1" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1869,61 +1878,61 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="36" customFormat="1" ht="34">
-      <c r="A5" s="36" t="s">
+    <row r="5" spans="1:33" s="35" customFormat="1" ht="34">
+      <c r="A5" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="R5" s="36" t="s">
+      <c r="R5" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="S5" s="36" t="s">
+      <c r="S5" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="Y5" s="36" t="s">
+      <c r="Y5" s="35" t="s">
         <v>183</v>
       </c>
       <c r="AA5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="36" customFormat="1" ht="17">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:33" s="35" customFormat="1" ht="17">
+      <c r="A6" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="36" t="s">
+      <c r="X6" s="35" t="s">
         <v>190</v>
       </c>
       <c r="AA6"/>
@@ -1972,7 +1981,7 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="40" t="s">
         <v>46</v>
       </c>
       <c r="C9" t="s">
@@ -1986,7 +1995,7 @@
       <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>192</v>
       </c>
       <c r="C10" t="s">
@@ -2024,7 +2033,7 @@
       <c r="A11" t="s">
         <v>194</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>195</v>
       </c>
       <c r="AB11" t="s">
@@ -2038,7 +2047,7 @@
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C12" t="s">
@@ -2049,7 +2058,7 @@
       <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C13" t="s">
@@ -2104,7 +2113,7 @@
       <c r="A15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="39" t="s">
         <v>192</v>
       </c>
       <c r="C15" t="s">
@@ -2121,7 +2130,7 @@
       <c r="A16" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C16" t="s">
@@ -2152,7 +2161,7 @@
       <c r="A18" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>46</v>
       </c>
       <c r="C18" t="s">
@@ -2166,7 +2175,7 @@
       <c r="A19" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>46</v>
       </c>
       <c r="C19" t="s">
@@ -2175,32 +2184,33 @@
       <c r="E19" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:31" s="27" customFormat="1">
-      <c r="A20" s="27" t="s">
+      <c r="Z19" s="1"/>
+    </row>
+    <row r="20" spans="1:31" s="26" customFormat="1">
+      <c r="A20" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:31" s="27" customFormat="1">
-      <c r="A21" s="27" t="s">
+    <row r="21" spans="1:31" s="26" customFormat="1">
+      <c r="A21" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="26" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2208,7 +2218,7 @@
       <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C22" t="s">
@@ -2264,7 +2274,7 @@
       <c r="A23" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>46</v>
       </c>
       <c r="C23" t="s">
@@ -2275,7 +2285,7 @@
       <c r="A24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C24" t="s">
@@ -2292,7 +2302,7 @@
       <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C25" t="s">
@@ -2309,7 +2319,7 @@
       <c r="A26" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C26" t="s">
@@ -2344,7 +2354,7 @@
       <c r="A27" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="26"/>
+      <c r="B27" s="25"/>
       <c r="C27" t="s">
         <v>167</v>
       </c>
@@ -2356,7 +2366,7 @@
       <c r="A28" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="32"/>
+      <c r="B28" s="31"/>
       <c r="C28" t="s">
         <v>119</v>
       </c>
@@ -2398,7 +2408,7 @@
       <c r="A29" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="15"/>
       <c r="C29" t="s">
         <v>93</v>
       </c>
@@ -2422,7 +2432,7 @@
       <c r="A30" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="16"/>
       <c r="C30" t="s">
         <v>93</v>
       </c>
@@ -2446,7 +2456,7 @@
       <c r="A31" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="18"/>
+      <c r="B31" s="17"/>
       <c r="C31" t="s">
         <v>93</v>
       </c>
@@ -2470,7 +2480,7 @@
       <c r="A32" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="33"/>
       <c r="C32" t="s">
         <v>168</v>
       </c>
@@ -2488,7 +2498,7 @@
       <c r="A33" t="s">
         <v>136</v>
       </c>
-      <c r="B33" s="33"/>
+      <c r="B33" s="32"/>
       <c r="C33" t="s">
         <v>138</v>
       </c>
@@ -2503,7 +2513,7 @@
       <c r="A34" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="18"/>
       <c r="C34" t="s">
         <v>94</v>
       </c>
@@ -2521,7 +2531,7 @@
       <c r="A35" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="19"/>
       <c r="C35" t="s">
         <v>94</v>
       </c>
@@ -2539,7 +2549,7 @@
       <c r="A36" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="18"/>
+      <c r="B36" s="17"/>
       <c r="C36" t="s">
         <v>94</v>
       </c>
@@ -2553,36 +2563,36 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:31" s="22" customFormat="1" ht="51">
-      <c r="A37" s="22" t="s">
+    <row r="37" spans="1:31" s="21" customFormat="1" ht="51">
+      <c r="A37" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="J37" s="22" t="s">
+      <c r="B37" s="22"/>
+      <c r="J37" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="L37" s="22" t="s">
+      <c r="L37" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="P37" s="22" t="s">
+      <c r="P37" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="R37" s="22" t="s">
+      <c r="R37" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="U37" s="22" t="s">
+      <c r="U37" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="X37" s="22" t="s">
+      <c r="X37" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="Y37" s="22" t="s">
+      <c r="Y37" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="AC37" s="22" t="s">
+      <c r="AC37" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="AE37" s="22" t="s">
+      <c r="AE37" s="21" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tidy up selection view
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E333F3-D0BB-2A47-BF97-DE43BFD93748}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E69459-4CCC-8540-9135-668E33C65DFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="1040" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="19820" yWindow="1640" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Storyboards" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="214">
   <si>
     <t>Storyboard</t>
   </si>
@@ -696,12 +696,21 @@
   <si>
     <t>Use a 20% alpha if override button is disabled (no changes)</t>
   </si>
+  <si>
+    <t>Shape Tabel Leg</t>
+  </si>
+  <si>
+    <t>Shape Table Leg Shadow</t>
+  </si>
+  <si>
+    <t>Thumbnail placeholder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -795,8 +804,15 @@
       <color rgb="FFE6BF5F"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFEFEFEC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="25">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -938,6 +954,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5AA8AB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7BDAC7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF75CDBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCEEEA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF75CCBC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -963,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1020,9 +1060,6 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1079,6 +1116,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1089,16 +1139,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEFEFEC"/>
+      <color rgb="FF75CCBC"/>
+      <color rgb="FFDCEEEA"/>
+      <color rgb="FF75CDBC"/>
+      <color rgb="FF7BDAC7"/>
       <color rgb="FF5AA8AB"/>
       <color rgb="FF9FE3AB"/>
       <color rgb="FFACFAD6"/>
       <color rgb="FFE6BF5F"/>
       <color rgb="FF7F7F80"/>
-      <color rgb="FFF1E5C9"/>
-      <color rgb="FF999999"/>
-      <color rgb="FFBFBFBF"/>
-      <color rgb="FF80807E"/>
-      <color rgb="FFE7E5E8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1591,18 +1641,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
-  <dimension ref="A1:AG37"/>
+  <dimension ref="A1:AG40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB16" sqref="AB16"/>
+      <selection pane="bottomRight" activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
@@ -1878,61 +1928,61 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="35" customFormat="1" ht="34">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:33" s="34" customFormat="1" ht="34">
+      <c r="A5" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="R5" s="35" t="s">
+      <c r="R5" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="Y5" s="35" t="s">
+      <c r="Y5" s="34" t="s">
         <v>183</v>
       </c>
       <c r="AA5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="35" customFormat="1" ht="17">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:33" s="34" customFormat="1" ht="17">
+      <c r="A6" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="35" t="s">
+      <c r="X6" s="34" t="s">
         <v>190</v>
       </c>
       <c r="AA6"/>
@@ -1981,7 +2031,7 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>46</v>
       </c>
       <c r="C9" t="s">
@@ -1995,7 +2045,7 @@
       <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>192</v>
       </c>
       <c r="C10" t="s">
@@ -2033,7 +2083,7 @@
       <c r="A11" t="s">
         <v>194</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="37" t="s">
         <v>195</v>
       </c>
       <c r="AB11" t="s">
@@ -2113,7 +2163,7 @@
       <c r="A15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="38" t="s">
         <v>192</v>
       </c>
       <c r="C15" t="s">
@@ -2130,7 +2180,7 @@
       <c r="A16" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="44" t="s">
         <v>46</v>
       </c>
       <c r="C16" t="s">
@@ -2145,37 +2195,31 @@
     </row>
     <row r="17" spans="1:31">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="43" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:31">
       <c r="A18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
+        <v>52</v>
+      </c>
+      <c r="I18" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:31">
       <c r="A19" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C19" t="s">
@@ -2184,415 +2228,441 @@
       <c r="E19" t="s">
         <v>68</v>
       </c>
-      <c r="Z19" s="1"/>
-    </row>
-    <row r="20" spans="1:31" s="26" customFormat="1">
-      <c r="A20" s="26" t="s">
+    </row>
+    <row r="20" spans="1:31">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" spans="1:31" s="25" customFormat="1">
+      <c r="A21" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E21" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:31" s="26" customFormat="1">
-      <c r="A21" s="26" t="s">
+    <row r="22" spans="1:31" s="25" customFormat="1">
+      <c r="A22" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E22" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" t="s">
-        <v>83</v>
-      </c>
-      <c r="J22" t="s">
-        <v>105</v>
-      </c>
-      <c r="M22" t="s">
-        <v>134</v>
-      </c>
-      <c r="R22" t="s">
-        <v>148</v>
-      </c>
-      <c r="T22" t="s">
-        <v>163</v>
-      </c>
-      <c r="V22" t="s">
-        <v>173</v>
-      </c>
-      <c r="W22" t="s">
-        <v>173</v>
-      </c>
-      <c r="X22" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>173</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>205</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31">
-      <c r="A23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>200</v>
-      </c>
+    <row r="23" spans="1:31" s="25" customFormat="1">
+      <c r="A23" s="40" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23" s="41"/>
+    </row>
+    <row r="24" spans="1:31" s="25" customFormat="1">
+      <c r="A24" s="40" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="42"/>
     </row>
     <row r="25" spans="1:31">
       <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="9" t="s">
         <v>46</v>
       </c>
+      <c r="B25" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" t="s">
+        <v>83</v>
       </c>
       <c r="J25" t="s">
-        <v>98</v>
+        <v>105</v>
+      </c>
+      <c r="M25" t="s">
+        <v>134</v>
+      </c>
+      <c r="R25" t="s">
+        <v>148</v>
+      </c>
+      <c r="T25" t="s">
+        <v>163</v>
+      </c>
+      <c r="V25" t="s">
+        <v>173</v>
+      </c>
+      <c r="W25" t="s">
+        <v>173</v>
       </c>
       <c r="X25" t="s">
-        <v>181</v>
+        <v>173</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:31">
       <c r="A26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" t="s">
-        <v>73</v>
-      </c>
-      <c r="O26" t="s">
-        <v>155</v>
-      </c>
-      <c r="P26" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>160</v>
-      </c>
-      <c r="T26" t="s">
-        <v>164</v>
-      </c>
-      <c r="X26" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:31">
       <c r="A27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="25"/>
+        <v>44</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="C27" t="s">
-        <v>167</v>
-      </c>
-      <c r="I27" t="s">
-        <v>123</v>
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:31">
       <c r="A28" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="31"/>
+        <v>45</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="C28" t="s">
-        <v>119</v>
-      </c>
-      <c r="H28" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="J28" t="s">
-        <v>126</v>
-      </c>
-      <c r="O28" t="s">
-        <v>156</v>
-      </c>
-      <c r="P28" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>157</v>
-      </c>
-      <c r="R28" t="s">
-        <v>147</v>
-      </c>
-      <c r="V28" t="s">
-        <v>172</v>
-      </c>
-      <c r="W28" t="s">
-        <v>178</v>
+        <v>98</v>
       </c>
       <c r="X28" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>209</v>
-      </c>
-      <c r="AE28" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:31">
       <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="15"/>
+        <v>71</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" t="s">
-        <v>95</v>
-      </c>
-      <c r="K29" t="s">
-        <v>128</v>
-      </c>
-      <c r="N29" t="s">
-        <v>153</v>
-      </c>
-      <c r="R29" t="s">
-        <v>153</v>
+        <v>72</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+      <c r="O29" t="s">
+        <v>155</v>
+      </c>
+      <c r="P29" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>160</v>
+      </c>
+      <c r="T29" t="s">
+        <v>164</v>
+      </c>
+      <c r="X29" t="s">
+        <v>180</v>
       </c>
       <c r="AB29" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:31">
       <c r="A30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="16"/>
+        <v>122</v>
+      </c>
+      <c r="B30" s="24"/>
       <c r="C30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K30" t="s">
-        <v>128</v>
-      </c>
-      <c r="N30" t="s">
-        <v>153</v>
-      </c>
-      <c r="R30" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>198</v>
+        <v>167</v>
+      </c>
+      <c r="I30" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:31">
       <c r="A31" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="B31" s="30"/>
       <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" t="s">
-        <v>95</v>
-      </c>
-      <c r="K31" t="s">
-        <v>128</v>
-      </c>
-      <c r="N31" t="s">
-        <v>153</v>
+        <v>119</v>
+      </c>
+      <c r="H31" t="s">
+        <v>120</v>
+      </c>
+      <c r="J31" t="s">
+        <v>126</v>
+      </c>
+      <c r="O31" t="s">
+        <v>156</v>
+      </c>
+      <c r="P31" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>157</v>
       </c>
       <c r="R31" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>198</v>
+        <v>147</v>
+      </c>
+      <c r="V31" t="s">
+        <v>172</v>
+      </c>
+      <c r="W31" t="s">
+        <v>178</v>
+      </c>
+      <c r="X31" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:31">
       <c r="A32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" s="33"/>
+        <v>87</v>
+      </c>
+      <c r="B32" s="15"/>
       <c r="C32" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
+        <v>95</v>
+      </c>
+      <c r="K32" t="s">
+        <v>128</v>
       </c>
       <c r="N32" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="R32" t="s">
-        <v>143</v>
+        <v>153</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:31">
       <c r="A33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B33" s="32"/>
+        <v>88</v>
+      </c>
+      <c r="B33" s="16"/>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>95</v>
+      </c>
+      <c r="K33" t="s">
+        <v>128</v>
       </c>
       <c r="N33" t="s">
-        <v>138</v>
+        <v>153</v>
+      </c>
+      <c r="R33" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:31">
       <c r="A34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="18"/>
+        <v>92</v>
+      </c>
+      <c r="B34" s="17"/>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K34" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="N34" t="s">
+        <v>153</v>
       </c>
       <c r="R34" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:31">
       <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="B35" s="32"/>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
-      </c>
-      <c r="K35" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="N35" t="s">
+        <v>139</v>
       </c>
       <c r="R35" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:31">
       <c r="A36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" t="s">
+        <v>138</v>
+      </c>
+      <c r="N36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+      <c r="K37" t="s">
+        <v>129</v>
+      </c>
+      <c r="R37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+      <c r="K38" t="s">
+        <v>129</v>
+      </c>
+      <c r="R38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31">
+      <c r="A39" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" t="s">
         <v>94</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D39" t="s">
         <v>96</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K39" t="s">
         <v>129</v>
       </c>
-      <c r="R36" t="s">
+      <c r="R39" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:31" s="21" customFormat="1" ht="51">
-      <c r="A37" s="21" t="s">
+    <row r="40" spans="1:31" s="20" customFormat="1" ht="51">
+      <c r="A40" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="J37" s="21" t="s">
+      <c r="B40" s="21"/>
+      <c r="J40" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="L37" s="21" t="s">
+      <c r="L40" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="P37" s="21" t="s">
+      <c r="P40" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="R37" s="21" t="s">
+      <c r="R40" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="U37" s="21" t="s">
+      <c r="U40" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="X37" s="21" t="s">
+      <c r="X40" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="Y37" s="21" t="s">
+      <c r="Y40" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="AC37" s="21" t="s">
+      <c r="AC40" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="AE37" s="21" t="s">
+      <c r="AE40" s="20" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New version of client
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E69459-4CCC-8540-9135-668E33C65DFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B85F8E-9E12-204C-BD1E-46C91DADCE84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19820" yWindow="1640" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="17520" yWindow="2400" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Storyboards" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="216">
   <si>
     <t>Storyboard</t>
   </si>
@@ -705,12 +705,18 @@
   <si>
     <t>Thumbnail placeholder</t>
   </si>
+  <si>
+    <t>Continue Button</t>
+  </si>
+  <si>
+    <t>Room Interior</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -811,8 +817,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -978,6 +991,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF75CCBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF74B374"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1003,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1129,6 +1148,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1140,6 +1165,7 @@
   <colors>
     <mruColors>
       <color rgb="FFEFEFEC"/>
+      <color rgb="FF74B374"/>
       <color rgb="FF75CCBC"/>
       <color rgb="FFDCEEEA"/>
       <color rgb="FF75CDBC"/>
@@ -1148,7 +1174,6 @@
       <color rgb="FF9FE3AB"/>
       <color rgb="FFACFAD6"/>
       <color rgb="FFE6BF5F"/>
-      <color rgb="FF7F7F80"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1641,13 +1666,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
-  <dimension ref="A1:AG40"/>
+  <dimension ref="A1:AG42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z24" sqref="Z24"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1841,7 +1866,7 @@
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C3" t="s">
@@ -1928,605 +1953,579 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="34" customFormat="1" ht="34">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:33">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" s="34" customFormat="1" ht="34">
+      <c r="A6" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B6" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C6" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D6" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F6" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G6" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H6" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J6" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K6" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="34" t="s">
+      <c r="L6" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="N6" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="R5" s="34" t="s">
+      <c r="R6" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="S5" s="34" t="s">
+      <c r="S6" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="Y5" s="34" t="s">
+      <c r="Y6" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AA6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="34" customFormat="1" ht="17">
-      <c r="A6" s="34" t="s">
+    <row r="7" spans="1:33" s="34" customFormat="1" ht="17">
+      <c r="A7" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B7" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="34" t="s">
+      <c r="X7" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:33">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" t="s">
-        <v>106</v>
-      </c>
+      <c r="AA7"/>
     </row>
     <row r="8" spans="1:33">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:33">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="R9" t="s">
-        <v>144</v>
+        <v>62</v>
+      </c>
+      <c r="I9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:33">
       <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>192</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
       <c r="R10" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>184</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:33">
       <c r="A11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>197</v>
+        <v>39</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>159</v>
+      </c>
+      <c r="R11" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>184</v>
       </c>
       <c r="AD11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:33">
       <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>65</v>
+        <v>194</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:33">
       <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
-      </c>
-      <c r="O13" t="s">
-        <v>165</v>
-      </c>
-      <c r="P13" t="s">
-        <v>165</v>
-      </c>
-      <c r="T13" t="s">
-        <v>165</v>
-      </c>
-      <c r="V13" t="s">
-        <v>174</v>
-      </c>
-      <c r="W13" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>187</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>165</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>165</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:33">
       <c r="A14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="39" t="s">
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>196</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>208</v>
+        <v>63</v>
+      </c>
+      <c r="R14" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:33">
       <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>192</v>
+        <v>41</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="R15" t="s">
-        <v>145</v>
-      </c>
-      <c r="S15" t="s">
-        <v>162</v>
+        <v>53</v>
+      </c>
+      <c r="O15" t="s">
+        <v>165</v>
+      </c>
+      <c r="P15" t="s">
+        <v>165</v>
+      </c>
+      <c r="T15" t="s">
+        <v>165</v>
+      </c>
+      <c r="V15" t="s">
+        <v>174</v>
+      </c>
+      <c r="W15" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:33">
       <c r="A16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" t="s">
-        <v>101</v>
-      </c>
-      <c r="U16" t="s">
-        <v>170</v>
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:31">
       <c r="A17" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="R17" t="s">
+        <v>145</v>
+      </c>
+      <c r="S17" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:31">
       <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="44" t="s">
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" t="s">
-        <v>86</v>
+        <v>117</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="U18" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:31">
       <c r="A19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="43" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:31">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
+      <c r="A22" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B22" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" t="s">
         <v>68</v>
       </c>
-      <c r="Z20" s="1"/>
-    </row>
-    <row r="21" spans="1:31" s="25" customFormat="1">
-      <c r="A21" s="25" t="s">
+      <c r="Z22" s="1"/>
+    </row>
+    <row r="23" spans="1:31" s="25" customFormat="1">
+      <c r="A23" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B23" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C23" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E23" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:31" s="25" customFormat="1">
-      <c r="A22" s="25" t="s">
+    <row r="24" spans="1:31" s="25" customFormat="1">
+      <c r="A24" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B24" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C24" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E24" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:31" s="25" customFormat="1">
-      <c r="A23" s="40" t="s">
+    <row r="25" spans="1:31" s="25" customFormat="1">
+      <c r="A25" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="B23" s="41"/>
-    </row>
-    <row r="24" spans="1:31" s="25" customFormat="1">
-      <c r="A24" s="40" t="s">
+      <c r="B25" s="41"/>
+    </row>
+    <row r="26" spans="1:31" s="25" customFormat="1">
+      <c r="A26" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="B24" s="42"/>
-    </row>
-    <row r="25" spans="1:31">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" t="s">
-        <v>83</v>
-      </c>
-      <c r="J25" t="s">
-        <v>105</v>
-      </c>
-      <c r="M25" t="s">
-        <v>134</v>
-      </c>
-      <c r="R25" t="s">
-        <v>148</v>
-      </c>
-      <c r="T25" t="s">
-        <v>163</v>
-      </c>
-      <c r="V25" t="s">
-        <v>173</v>
-      </c>
-      <c r="W25" t="s">
-        <v>173</v>
-      </c>
-      <c r="X25" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>173</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>205</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31">
-      <c r="A26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>166</v>
-      </c>
+      <c r="B26" s="42"/>
     </row>
     <row r="27" spans="1:31">
       <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="22" t="s">
         <v>46</v>
       </c>
+      <c r="B27" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" t="s">
+        <v>105</v>
+      </c>
+      <c r="M27" t="s">
+        <v>134</v>
+      </c>
+      <c r="R27" t="s">
+        <v>148</v>
+      </c>
+      <c r="T27" t="s">
+        <v>163</v>
+      </c>
+      <c r="V27" t="s">
+        <v>173</v>
+      </c>
+      <c r="W27" t="s">
+        <v>173</v>
+      </c>
+      <c r="X27" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>173</v>
       </c>
       <c r="AC27" t="s">
-        <v>200</v>
+        <v>202</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:31">
       <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
-      </c>
-      <c r="J28" t="s">
-        <v>98</v>
-      </c>
-      <c r="X28" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:31">
       <c r="A29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" t="s">
-        <v>73</v>
-      </c>
-      <c r="O29" t="s">
-        <v>155</v>
-      </c>
-      <c r="P29" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>160</v>
-      </c>
-      <c r="T29" t="s">
-        <v>164</v>
-      </c>
-      <c r="X29" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>199</v>
+        <v>70</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:31">
       <c r="A30" t="s">
-        <v>122</v>
-      </c>
-      <c r="B30" s="24"/>
+        <v>45</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="C30" t="s">
-        <v>167</v>
-      </c>
-      <c r="I30" t="s">
-        <v>123</v>
+        <v>51</v>
+      </c>
+      <c r="J30" t="s">
+        <v>98</v>
+      </c>
+      <c r="X30" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:31">
       <c r="A31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="30"/>
+        <v>71</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C31" t="s">
-        <v>119</v>
-      </c>
-      <c r="H31" t="s">
-        <v>120</v>
-      </c>
-      <c r="J31" t="s">
-        <v>126</v>
+        <v>72</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
       </c>
       <c r="O31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q31" t="s">
-        <v>157</v>
-      </c>
-      <c r="R31" t="s">
-        <v>147</v>
-      </c>
-      <c r="V31" t="s">
-        <v>172</v>
-      </c>
-      <c r="W31" t="s">
-        <v>178</v>
+        <v>160</v>
+      </c>
+      <c r="T31" t="s">
+        <v>164</v>
       </c>
       <c r="X31" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>209</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>209</v>
+        <v>180</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:31">
       <c r="A32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" s="15"/>
+        <v>122</v>
+      </c>
+      <c r="B32" s="24"/>
       <c r="C32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" t="s">
-        <v>95</v>
-      </c>
-      <c r="K32" t="s">
-        <v>128</v>
-      </c>
-      <c r="N32" t="s">
-        <v>153</v>
-      </c>
-      <c r="R32" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>198</v>
+        <v>167</v>
+      </c>
+      <c r="I32" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:31">
       <c r="A33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="16"/>
+        <v>118</v>
+      </c>
+      <c r="B33" s="30"/>
       <c r="C33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="K33" t="s">
-        <v>128</v>
-      </c>
-      <c r="N33" t="s">
-        <v>153</v>
+        <v>119</v>
+      </c>
+      <c r="H33" t="s">
+        <v>120</v>
+      </c>
+      <c r="J33" t="s">
+        <v>126</v>
+      </c>
+      <c r="O33" t="s">
+        <v>156</v>
+      </c>
+      <c r="P33" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>157</v>
       </c>
       <c r="R33" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>198</v>
+        <v>147</v>
+      </c>
+      <c r="V33" t="s">
+        <v>172</v>
+      </c>
+      <c r="W33" t="s">
+        <v>178</v>
+      </c>
+      <c r="X33" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:31">
       <c r="A34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="17"/>
+        <v>87</v>
+      </c>
+      <c r="B34" s="15"/>
       <c r="C34" t="s">
         <v>93</v>
       </c>
@@ -2548,78 +2547,90 @@
     </row>
     <row r="35" spans="1:31">
       <c r="A35" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="32"/>
+        <v>88</v>
+      </c>
+      <c r="B35" s="16"/>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>95</v>
+      </c>
+      <c r="K35" t="s">
+        <v>128</v>
       </c>
       <c r="N35" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="R35" t="s">
-        <v>143</v>
+        <v>153</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:31">
       <c r="A36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" s="31"/>
+        <v>92</v>
+      </c>
+      <c r="B36" s="17"/>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>138</v>
+        <v>95</v>
+      </c>
+      <c r="K36" t="s">
+        <v>128</v>
       </c>
       <c r="N36" t="s">
-        <v>138</v>
+        <v>153</v>
+      </c>
+      <c r="R36" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:31">
       <c r="A37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="18"/>
+        <v>135</v>
+      </c>
+      <c r="B37" s="32"/>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
-      </c>
-      <c r="K37" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="N37" t="s">
+        <v>139</v>
       </c>
       <c r="R37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:31">
       <c r="A38" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="19"/>
+        <v>136</v>
+      </c>
+      <c r="B38" s="31"/>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K38" t="s">
-        <v>129</v>
-      </c>
-      <c r="R38" t="s">
-        <v>152</v>
+        <v>138</v>
+      </c>
+      <c r="N38" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:31">
       <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="17"/>
+        <v>90</v>
+      </c>
+      <c r="B39" s="18"/>
       <c r="C39" t="s">
         <v>94</v>
       </c>
@@ -2633,36 +2644,72 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:31" s="20" customFormat="1" ht="51">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:31">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+      <c r="K40" t="s">
+        <v>129</v>
+      </c>
+      <c r="R40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" t="s">
+        <v>96</v>
+      </c>
+      <c r="K41" t="s">
+        <v>129</v>
+      </c>
+      <c r="R41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" s="20" customFormat="1" ht="51">
+      <c r="A42" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="J40" s="20" t="s">
+      <c r="B42" s="21"/>
+      <c r="J42" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="L40" s="20" t="s">
+      <c r="L42" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="P40" s="20" t="s">
+      <c r="P42" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="R40" s="20" t="s">
+      <c r="R42" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="U40" s="20" t="s">
+      <c r="U42" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="X40" s="20" t="s">
+      <c r="X42" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="Y40" s="20" t="s">
+      <c r="Y42" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="AC40" s="20" t="s">
+      <c r="AC42" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="AE40" s="20" t="s">
+      <c r="AE42" s="20" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sort out View Game option Sort out Auto-play Sort out refresh after sync Sort out online game completion Make all popovers modal
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2289CA-46FF-024B-8D23-1C3F3FB8EB84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCE475E-D866-9348-8927-8D9FE040D003}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="3120" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Storyboards" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="228">
   <si>
     <t>Storyboard</t>
   </si>
@@ -446,12 +446,6 @@
   </si>
   <si>
     <t>Card back</t>
-  </si>
-  <si>
-    <t>Card back outline</t>
-  </si>
-  <si>
-    <t>Background / players / outcome</t>
   </si>
   <si>
     <t>Select Players</t>
@@ -713,6 +707,45 @@
   </si>
   <si>
     <t>Instruction</t>
+  </si>
+  <si>
+    <t>iPhone X</t>
+  </si>
+  <si>
+    <t>landscape</t>
+  </si>
+  <si>
+    <t>portrait</t>
+  </si>
+  <si>
+    <t>iPhone 7</t>
+  </si>
+  <si>
+    <t>iPhone SE</t>
+  </si>
+  <si>
+    <t>iPad</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Select opponents (host)</t>
+  </si>
+  <si>
+    <t>Select players</t>
+  </si>
+  <si>
+    <t>Single player</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>XXX  (cut?)</t>
   </si>
 </sst>
 </file>
@@ -828,7 +861,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1003,6 +1036,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1025,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1163,6 +1202,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1675,13 +1728,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
-  <dimension ref="A1:AE45"/>
+  <dimension ref="A1:AD58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1690,10 +1743,12 @@
     <col min="2" max="2" width="14.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="31" width="21.6640625" customWidth="1"/>
+    <col min="5" max="11" width="21.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="50" customWidth="1"/>
+    <col min="13" max="30" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="2" customFormat="1" ht="31" customHeight="1">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="31" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -1727,68 +1782,65 @@
       <c r="K1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="49" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>15</v>
+        <v>138</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>173</v>
+        <v>19</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1819,23 +1871,26 @@
       <c r="M2" t="s">
         <v>132</v>
       </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
       <c r="O2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q2" t="s">
         <v>30</v>
-      </c>
-      <c r="P2" t="s">
-        <v>141</v>
       </c>
       <c r="R2" t="s">
         <v>30</v>
       </c>
       <c r="S2" t="s">
+        <v>169</v>
+      </c>
+      <c r="T2" t="s">
+        <v>169</v>
+      </c>
+      <c r="U2" t="s">
         <v>30</v>
-      </c>
-      <c r="T2" t="s">
-        <v>171</v>
-      </c>
-      <c r="U2" t="s">
-        <v>171</v>
       </c>
       <c r="V2" t="s">
         <v>30</v>
@@ -1843,23 +1898,20 @@
       <c r="W2" t="s">
         <v>30</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>30</v>
       </c>
       <c r="Z2" t="s">
         <v>30</v>
       </c>
       <c r="AA2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1881,14 +1933,17 @@
       <c r="M3" t="s">
         <v>131</v>
       </c>
-      <c r="P3" t="s">
-        <v>149</v>
+      <c r="O3" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>103</v>
       </c>
       <c r="R3" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="S3" t="s">
-        <v>165</v>
+        <v>34</v>
       </c>
       <c r="T3" t="s">
         <v>34</v>
@@ -1900,31 +1955,28 @@
         <v>34</v>
       </c>
       <c r="W3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y3" t="s">
         <v>34</v>
-      </c>
-      <c r="X3" t="s">
-        <v>178</v>
       </c>
       <c r="Z3" t="s">
         <v>34</v>
       </c>
       <c r="AA3" t="s">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="AB3" t="s">
-        <v>199</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G4" t="s">
         <v>34</v>
@@ -1932,11 +1984,11 @@
       <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="O4" t="s">
+      <c r="N4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1946,21 +1998,21 @@
       <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="P5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31">
+      <c r="O5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B7" s="46" t="s">
         <v>46</v>
@@ -1969,12 +2021,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:31" s="33" customFormat="1" ht="34">
+    <row r="8" spans="1:30" s="33" customFormat="1" ht="34">
       <c r="A8" s="33" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>60</v>
@@ -1997,38 +2049,36 @@
       <c r="K8" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="N8" s="33" t="s">
-        <v>139</v>
+      <c r="O8" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="P8" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q8" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="W8" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" s="33" customFormat="1" ht="17">
+        <v>155</v>
+      </c>
+      <c r="V8" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="X8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" s="33" customFormat="1" ht="17">
       <c r="A9" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="V9" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y9"/>
-    </row>
-    <row r="10" spans="1:31">
+      <c r="L9" s="51"/>
+      <c r="U9" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="X9"/>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2045,9 +2095,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:30">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>46</v>
@@ -2056,7 +2106,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:30">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2073,7 +2123,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:30">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2083,16 +2133,16 @@
       <c r="C13" t="s">
         <v>63</v>
       </c>
-      <c r="P13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31">
+      <c r="O13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
         <v>64</v>
@@ -2109,31 +2159,31 @@
       <c r="I14" t="s">
         <v>123</v>
       </c>
-      <c r="P14" t="s">
-        <v>145</v>
-      </c>
-      <c r="W14" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="O14" t="s">
+        <v>143</v>
+      </c>
+      <c r="V14" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B15" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y15" t="s">
         <v>191</v>
       </c>
-      <c r="Z15" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31">
+      <c r="AA15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2144,9 +2194,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>46</v>
@@ -2157,11 +2207,11 @@
       <c r="I17" t="s">
         <v>85</v>
       </c>
-      <c r="P17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29">
+      <c r="O17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -2171,29 +2221,29 @@
       <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="O18" t="s">
-        <v>161</v>
-      </c>
-      <c r="R18" t="s">
-        <v>161</v>
+      <c r="N18" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>159</v>
+      </c>
+      <c r="S18" t="s">
+        <v>168</v>
       </c>
       <c r="T18" t="s">
-        <v>170</v>
-      </c>
-      <c r="U18" t="s">
-        <v>170</v>
-      </c>
-      <c r="W18" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>161</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29">
+        <v>168</v>
+      </c>
+      <c r="V18" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -2206,37 +2256,37 @@
       <c r="F19" t="s">
         <v>78</v>
       </c>
-      <c r="Z19" t="s">
-        <v>192</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29">
+      <c r="Y19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C20" t="s">
         <v>54</v>
       </c>
       <c r="I20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J20" t="s">
         <v>34</v>
       </c>
+      <c r="O20" t="s">
+        <v>142</v>
+      </c>
       <c r="P20" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -2249,19 +2299,19 @@
       <c r="D21" t="s">
         <v>100</v>
       </c>
-      <c r="S21" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29">
+      <c r="R21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2272,7 +2322,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
         <v>114</v>
       </c>
@@ -2286,7 +2336,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
         <v>115</v>
       </c>
@@ -2299,9 +2349,9 @@
       <c r="E25" t="s">
         <v>68</v>
       </c>
-      <c r="X25" s="1"/>
-    </row>
-    <row r="26" spans="1:29" s="25" customFormat="1">
+      <c r="W25" s="1"/>
+    </row>
+    <row r="26" spans="1:28" s="25" customFormat="1">
       <c r="A26" s="25" t="s">
         <v>42</v>
       </c>
@@ -2314,8 +2364,9 @@
       <c r="E26" s="25" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:29" s="25" customFormat="1">
+      <c r="L26" s="52"/>
+    </row>
+    <row r="27" spans="1:28" s="25" customFormat="1">
       <c r="A27" s="25" t="s">
         <v>113</v>
       </c>
@@ -2328,20 +2379,23 @@
       <c r="E27" s="25" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="1:29" s="25" customFormat="1">
+      <c r="L27" s="52"/>
+    </row>
+    <row r="28" spans="1:28" s="25" customFormat="1">
       <c r="A28" s="39" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B28" s="40"/>
-    </row>
-    <row r="29" spans="1:29" s="25" customFormat="1">
+      <c r="L28" s="52"/>
+    </row>
+    <row r="29" spans="1:28" s="25" customFormat="1">
       <c r="A29" s="39" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B29" s="41"/>
-    </row>
-    <row r="30" spans="1:29">
+      <c r="L29" s="52"/>
+    </row>
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2366,38 +2420,38 @@
       <c r="M30" t="s">
         <v>133</v>
       </c>
-      <c r="P30" t="s">
-        <v>147</v>
-      </c>
-      <c r="R30" t="s">
-        <v>159</v>
+      <c r="O30" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>157</v>
+      </c>
+      <c r="S30" t="s">
+        <v>167</v>
       </c>
       <c r="T30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V30" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="W30" t="s">
-        <v>181</v>
-      </c>
-      <c r="X30" t="s">
-        <v>169</v>
+        <v>167</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>196</v>
       </c>
       <c r="AA30" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AB30" t="s">
         <v>201</v>
       </c>
-      <c r="AC30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29">
+    </row>
+    <row r="31" spans="1:28">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2405,10 +2459,10 @@
         <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2421,11 +2475,11 @@
       <c r="E32" t="s">
         <v>70</v>
       </c>
-      <c r="AA32" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29">
+      <c r="Z32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2438,11 +2492,11 @@
       <c r="J33" t="s">
         <v>97</v>
       </c>
-      <c r="V33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29">
+      <c r="U33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2458,32 +2512,32 @@
       <c r="F34" t="s">
         <v>73</v>
       </c>
-      <c r="O34" t="s">
-        <v>154</v>
-      </c>
-      <c r="R34" t="s">
-        <v>160</v>
-      </c>
-      <c r="V34" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29">
+      <c r="N34" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>158</v>
+      </c>
+      <c r="U34" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30">
       <c r="A35" t="s">
         <v>121</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I35" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:30">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -2497,29 +2551,29 @@
       <c r="J36" t="s">
         <v>125</v>
       </c>
+      <c r="N36" t="s">
+        <v>153</v>
+      </c>
       <c r="O36" t="s">
-        <v>155</v>
-      </c>
-      <c r="P36" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="S36" t="s">
+        <v>166</v>
       </c>
       <c r="T36" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="U36" t="s">
-        <v>174</v>
-      </c>
-      <c r="V36" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>203</v>
       </c>
       <c r="AB36" t="s">
-        <v>205</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2533,17 +2587,14 @@
       <c r="K37" t="s">
         <v>127</v>
       </c>
-      <c r="N37" t="s">
-        <v>152</v>
-      </c>
-      <c r="P37" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="38" spans="1:29">
+      <c r="O37" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -2557,17 +2608,14 @@
       <c r="K38" t="s">
         <v>127</v>
       </c>
-      <c r="N38" t="s">
-        <v>152</v>
-      </c>
-      <c r="P38" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29">
+      <c r="O38" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -2581,35 +2629,29 @@
       <c r="K39" t="s">
         <v>127</v>
       </c>
-      <c r="N39" t="s">
-        <v>152</v>
-      </c>
-      <c r="P39" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z39" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="40" spans="1:29">
+      <c r="O39" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30">
       <c r="A40" t="s">
         <v>134</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D40" t="s">
         <v>136</v>
       </c>
-      <c r="N40" t="s">
-        <v>138</v>
-      </c>
-      <c r="P40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:29">
+      <c r="O40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30">
       <c r="A41" t="s">
         <v>135</v>
       </c>
@@ -2620,11 +2662,8 @@
       <c r="D41" t="s">
         <v>137</v>
       </c>
-      <c r="N41" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:29">
+    </row>
+    <row r="42" spans="1:30">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2638,11 +2677,11 @@
       <c r="K42" t="s">
         <v>128</v>
       </c>
-      <c r="P42" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:29">
+      <c r="O42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2656,11 +2695,11 @@
       <c r="K43" t="s">
         <v>128</v>
       </c>
-      <c r="P43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29">
+      <c r="O43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2674,11 +2713,11 @@
       <c r="K44" t="s">
         <v>128</v>
       </c>
-      <c r="P44" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:29" s="20" customFormat="1" ht="51">
+      <c r="O44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" s="20" customFormat="1" ht="51">
       <c r="A45" s="20" t="s">
         <v>109</v>
       </c>
@@ -2686,29 +2725,491 @@
       <c r="J45" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="L45" s="20" t="s">
+      <c r="L45" s="53" t="s">
         <v>130</v>
       </c>
+      <c r="N45" s="20" t="s">
+        <v>154</v>
+      </c>
       <c r="O45" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="P45" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="S45" s="20" t="s">
-        <v>167</v>
+        <v>148</v>
+      </c>
+      <c r="R45" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="U45" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="V45" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="W45" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA45" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC45" s="20" t="s">
-        <v>206</v>
+        <v>180</v>
+      </c>
+      <c r="Z45" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB45" s="20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30">
+      <c r="A48" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L48" s="54"/>
+      <c r="M48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3"/>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="3"/>
+    </row>
+    <row r="49" spans="1:30">
+      <c r="B49" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L49" s="54"/>
+      <c r="M49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="3"/>
+      <c r="AC49" s="3"/>
+      <c r="AD49" s="3"/>
+    </row>
+    <row r="50" spans="1:30">
+      <c r="A50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L50" s="54"/>
+      <c r="M50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P50" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3"/>
+      <c r="AC50" s="3"/>
+      <c r="AD50" s="3"/>
+    </row>
+    <row r="51" spans="1:30">
+      <c r="B51" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L51" s="54"/>
+      <c r="M51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="3"/>
+    </row>
+    <row r="52" spans="1:30">
+      <c r="A52" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L52" s="54"/>
+      <c r="M52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3"/>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3"/>
+      <c r="AC52" s="3"/>
+      <c r="AD52" s="3"/>
+    </row>
+    <row r="53" spans="1:30">
+      <c r="B53" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L53" s="54"/>
+      <c r="M53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="3"/>
+      <c r="Y53" s="3"/>
+      <c r="Z53" s="3"/>
+      <c r="AA53" s="3"/>
+      <c r="AB53" s="3"/>
+      <c r="AC53" s="3"/>
+      <c r="AD53" s="3"/>
+    </row>
+    <row r="54" spans="1:30">
+      <c r="A54" t="s">
+        <v>220</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L54" s="54"/>
+      <c r="M54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
+      <c r="W54" s="3"/>
+      <c r="X54" s="3"/>
+      <c r="Y54" s="3"/>
+      <c r="Z54" s="3"/>
+      <c r="AA54" s="3"/>
+      <c r="AB54" s="3"/>
+      <c r="AC54" s="3"/>
+      <c r="AD54" s="3"/>
+    </row>
+    <row r="55" spans="1:30">
+      <c r="B55" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L55" s="54"/>
+      <c r="M55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P55" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
+      <c r="X55" s="3"/>
+      <c r="Y55" s="3"/>
+      <c r="Z55" s="3"/>
+      <c r="AA55" s="3"/>
+      <c r="AB55" s="3"/>
+      <c r="AC55" s="3"/>
+      <c r="AD55" s="3"/>
+    </row>
+    <row r="56" spans="1:30">
+      <c r="G56" t="s">
+        <v>223</v>
+      </c>
+      <c r="H56" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30">
+      <c r="G57" t="s">
+        <v>224</v>
+      </c>
+      <c r="H57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30">
+      <c r="G58" t="s">
+        <v>225</v>
+      </c>
+      <c r="H58" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Good version of dashboards
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D7DFEB-79AB-CF45-8576-1CEA5A74AF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC6A2B-0B7E-6E49-B379-1E9B8DA79A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49200" yWindow="3120" windowWidth="23580" windowHeight="17440" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="40420" yWindow="560" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="2" r:id="rId1"/>
+    <sheet name="Views" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="236">
   <si>
     <t>Welcome</t>
   </si>
@@ -742,12 +745,61 @@
       <t xml:space="preserve"> Contrast</t>
     </r>
   </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Launch Screen</t>
+  </si>
+  <si>
+    <t>Confirm Played</t>
+  </si>
+  <si>
+    <t>Related Players</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
+  </si>
+  <si>
+    <t>Modernised</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Landscape</t>
+  </si>
+  <si>
+    <t>Portrait</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Specified</t>
+  </si>
+  <si>
+    <t>Waiting button re-design</t>
+  </si>
+  <si>
+    <t>Waiting for...</t>
+  </si>
+  <si>
+    <t>Dancing images, 
+disc images, 
+shield definitions, 
+rosette image, 
+trophy image</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -859,6 +911,13 @@
       <sz val="12"/>
       <color rgb="FF3B7F78"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="31">
@@ -1043,7 +1102,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1060,11 +1119,264 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1218,11 +1530,268 @@
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1548,11 +2117,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
   <dimension ref="A1:AD58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3034,4 +3603,715 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD168BF6-7604-814B-8525-59664C788955}">
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" style="55" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1">
+      <c r="A1" s="61"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="66"/>
+      <c r="F1" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="G1" s="66"/>
+      <c r="H1" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="58"/>
+      <c r="J1" s="79"/>
+    </row>
+    <row r="2" spans="1:10" s="56" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A2" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="I2" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="J2" s="80" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16" customHeight="1">
+      <c r="A3" s="83" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="89" t="str">
+        <f t="shared" ref="J3:J6" si="0">IF(B3="","Waiting for spec","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16" customHeight="1">
+      <c r="A4" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16" customHeight="1">
+      <c r="A5" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="84"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16" customHeight="1">
+      <c r="A6" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="84"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" customHeight="1">
+      <c r="A7" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="84"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="89" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" customHeight="1">
+      <c r="A8" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89" t="str">
+        <f t="shared" ref="J8:J9" si="1">IF(B8="","Waiting for spec","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16" customHeight="1">
+      <c r="A9" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="84"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89" t="str">
+        <f t="shared" si="1"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16" customHeight="1">
+      <c r="A10" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="89" t="str">
+        <f t="shared" ref="J9:J31" si="2">IF(B10="","Waiting for spec","")</f>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16" customHeight="1">
+      <c r="A11" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16" customHeight="1">
+      <c r="A12" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16" customHeight="1">
+      <c r="A13" s="83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16" customHeight="1">
+      <c r="A14" s="83" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" s="84"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" customHeight="1">
+      <c r="A15" s="83" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16" customHeight="1">
+      <c r="A16" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D16" s="85"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="88"/>
+      <c r="J16" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16" customHeight="1">
+      <c r="A17" s="83" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C17" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" s="85"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="89" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="85">
+      <c r="A18" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C18" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D18" s="85"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="89" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16" customHeight="1">
+      <c r="A19" s="83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D19" s="85"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="89" t="str">
+        <f t="shared" ref="J19:J31" si="3">IF(B19="","Waiting for spec","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16" customHeight="1">
+      <c r="A20" s="83" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C20" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="16" customHeight="1">
+      <c r="A21" s="83" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="85"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="16" customHeight="1">
+      <c r="A22" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="88"/>
+      <c r="J22" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16" customHeight="1">
+      <c r="A23" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="16" customHeight="1">
+      <c r="A24" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="85"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16" customHeight="1">
+      <c r="A25" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16" customHeight="1">
+      <c r="A26" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D26" s="85"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="16" customHeight="1">
+      <c r="A27" s="83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="84"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="16" customHeight="1">
+      <c r="A28" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="16" customHeight="1">
+      <c r="A29" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" s="85"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="88"/>
+      <c r="J29" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="16" customHeight="1">
+      <c r="A30" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="16" customHeight="1" thickBot="1">
+      <c r="A31" s="90" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="95"/>
+      <c r="J31" s="89" t="str">
+        <f t="shared" si="3"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" thickBot="1">
+      <c r="A32" s="71">
+        <f t="shared" ref="A32" si="4">COUNTIF(A3:A31, "&lt;&gt;")</f>
+        <v>29</v>
+      </c>
+      <c r="B32" s="72">
+        <f t="shared" ref="B32:I32" si="5">COUNTIF(B3:B31, "&lt;&gt;")</f>
+        <v>17</v>
+      </c>
+      <c r="C32" s="72">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="D32" s="69">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="73">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="69">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="73">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="69">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="70">
+        <f t="shared" ref="I32:J32" si="6">COUNTIF(I3:I31, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="81"/>
+    </row>
+    <row r="33" spans="1:10" ht="17" thickBot="1">
+      <c r="A33" s="75"/>
+      <c r="B33" s="74">
+        <f t="shared" ref="B33:I33" si="7">B32/$A32</f>
+        <v>0.58620689655172409</v>
+      </c>
+      <c r="C33" s="74">
+        <f t="shared" si="7"/>
+        <v>0.44827586206896552</v>
+      </c>
+      <c r="D33" s="76">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="77">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="76">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="77">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="76">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="78">
+        <f t="shared" ref="I33:J33" si="8">I32/$A32</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="82"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A3:J18 A19:I31">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND($B3="Yes", $C3="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:J31">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($B19="Yes", $C19="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working version of selection and preview
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC6A2B-0B7E-6E49-B379-1E9B8DA79A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ED770D-169A-A64B-B7B0-EFCB90932800}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40420" yWindow="560" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="236">
   <si>
     <t>Welcome</t>
   </si>
@@ -3610,7 +3610,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3718,7 +3718,9 @@
       <c r="B5" s="84" t="s">
         <v>231</v>
       </c>
-      <c r="C5" s="84"/>
+      <c r="C5" s="84" t="s">
+        <v>231</v>
+      </c>
       <c r="D5" s="85"/>
       <c r="E5" s="86"/>
       <c r="F5" s="85"/>
@@ -4231,7 +4233,7 @@
       </c>
       <c r="C32" s="72">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D32" s="69">
         <f t="shared" si="5"/>
@@ -4267,7 +4269,7 @@
       </c>
       <c r="C33" s="74">
         <f t="shared" si="7"/>
-        <v>0.44827586206896552</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="D33" s="76">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Tidied up Entry - introduced landscape view
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCECE13-E3C2-4C4C-89EF-6938BA933CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA30887D-35C0-9845-BD06-0EB962695468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40420" yWindow="560" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="235">
   <si>
     <t>Welcome</t>
   </si>
@@ -780,9 +780,6 @@
   </si>
   <si>
     <t>Specified</t>
-  </si>
-  <si>
-    <t>Waiting button re-design</t>
   </si>
   <si>
     <t>Waiting for...</t>
@@ -3490,7 +3487,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3546,7 +3543,7 @@
         <v>230</v>
       </c>
       <c r="J2" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1">
@@ -3649,9 +3646,7 @@
       <c r="G7" s="82"/>
       <c r="H7" s="83"/>
       <c r="I7" s="84"/>
-      <c r="J7" s="85" t="s">
-        <v>233</v>
-      </c>
+      <c r="J7" s="85"/>
     </row>
     <row r="8" spans="1:10" ht="16" customHeight="1">
       <c r="A8" s="79" t="s">
@@ -3660,7 +3655,9 @@
       <c r="B8" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="C8" s="80"/>
+      <c r="C8" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D8" s="81"/>
       <c r="E8" s="82"/>
       <c r="F8" s="81"/>
@@ -3854,7 +3851,7 @@
       <c r="H18" s="83"/>
       <c r="I18" s="84"/>
       <c r="J18" s="85" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1">
@@ -4117,7 +4114,7 @@
       </c>
       <c r="C32" s="68">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="65">
         <f t="shared" si="5"/>
@@ -4153,7 +4150,7 @@
       </c>
       <c r="C33" s="70">
         <f t="shared" si="7"/>
-        <v>0.55172413793103448</v>
+        <v>0.58620689655172409</v>
       </c>
       <c r="D33" s="72">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Additional work on various views
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA30887D-35C0-9845-BD06-0EB962695468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E074E6C1-A926-7E48-88A5-A75CCFF618FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40420" yWindow="560" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="238">
   <si>
     <t>Welcome</t>
   </si>
@@ -785,11 +785,16 @@
     <t>Waiting for...</t>
   </si>
   <si>
-    <t>Dancing images, 
-disc images, 
-shield definitions, 
-rosette image, 
-trophy image</t>
+    <t>Check colors with Jack</t>
+  </si>
+  <si>
+    <t>Check with Jack</t>
+  </si>
+  <si>
+    <t>Check size with Jack</t>
+  </si>
+  <si>
+    <t>Shield definitions</t>
   </si>
 </sst>
 </file>
@@ -3487,7 +3492,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3707,17 +3712,20 @@
       <c r="A11" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
+      <c r="B11" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D11" s="81"/>
       <c r="E11" s="82"/>
       <c r="F11" s="81"/>
       <c r="G11" s="82"/>
       <c r="H11" s="83"/>
       <c r="I11" s="84"/>
-      <c r="J11" s="85" t="str">
-        <f t="shared" si="2"/>
-        <v>Waiting for spec</v>
+      <c r="J11" s="85" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1">
@@ -3762,34 +3770,40 @@
       <c r="A14" s="79" t="s">
         <v>223</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
+      <c r="B14" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D14" s="81"/>
       <c r="E14" s="82"/>
       <c r="F14" s="81"/>
       <c r="G14" s="82"/>
       <c r="H14" s="83"/>
       <c r="I14" s="84"/>
-      <c r="J14" s="85" t="str">
-        <f t="shared" si="2"/>
-        <v>Waiting for spec</v>
+      <c r="J14" s="85" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1">
       <c r="A15" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
+      <c r="B15" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D15" s="81"/>
       <c r="E15" s="82"/>
       <c r="F15" s="81"/>
       <c r="G15" s="82"/>
       <c r="H15" s="83"/>
       <c r="I15" s="84"/>
-      <c r="J15" s="85" t="str">
-        <f t="shared" si="2"/>
-        <v>Waiting for spec</v>
+      <c r="J15" s="85" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1">
@@ -3834,7 +3848,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="85">
+    <row r="18" spans="1:10" ht="17">
       <c r="A18" s="79" t="s">
         <v>225</v>
       </c>
@@ -3851,7 +3865,7 @@
       <c r="H18" s="83"/>
       <c r="I18" s="84"/>
       <c r="J18" s="85" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1">
@@ -3942,17 +3956,20 @@
       <c r="A23" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
+      <c r="B23" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="C23" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D23" s="81"/>
       <c r="E23" s="82"/>
       <c r="F23" s="81"/>
       <c r="G23" s="82"/>
       <c r="H23" s="83"/>
       <c r="I23" s="84"/>
-      <c r="J23" s="85" t="str">
-        <f t="shared" si="3"/>
-        <v>Waiting for spec</v>
+      <c r="J23" s="85" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1">
@@ -3980,17 +3997,20 @@
       <c r="A25" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
+      <c r="B25" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="C25" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D25" s="81"/>
       <c r="E25" s="82"/>
       <c r="F25" s="81"/>
       <c r="G25" s="82"/>
       <c r="H25" s="83"/>
       <c r="I25" s="84"/>
-      <c r="J25" s="85" t="str">
-        <f t="shared" si="3"/>
-        <v>Waiting for spec</v>
+      <c r="J25" s="85" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1">
@@ -4035,8 +4055,12 @@
       <c r="A28" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="80"/>
-      <c r="C28" s="80"/>
+      <c r="B28" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="C28" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D28" s="81"/>
       <c r="E28" s="82"/>
       <c r="F28" s="81"/>
@@ -4045,7 +4069,7 @@
       <c r="I28" s="84"/>
       <c r="J28" s="85" t="str">
         <f t="shared" si="3"/>
-        <v>Waiting for spec</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1">
@@ -4064,9 +4088,8 @@
       <c r="G29" s="82"/>
       <c r="H29" s="83"/>
       <c r="I29" s="84"/>
-      <c r="J29" s="85" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="J29" s="85" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1">
@@ -4110,11 +4133,11 @@
       </c>
       <c r="B32" s="68">
         <f t="shared" ref="B32:H32" si="5">COUNTIF(B3:B31, "&lt;&gt;")</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C32" s="68">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D32" s="65">
         <f t="shared" si="5"/>
@@ -4146,11 +4169,11 @@
       <c r="A33" s="71"/>
       <c r="B33" s="70">
         <f t="shared" ref="B33:H33" si="7">B32/$A32</f>
-        <v>0.58620689655172409</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="C33" s="70">
         <f t="shared" si="7"/>
-        <v>0.58620689655172409</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="D33" s="72">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Initial implementation of awards
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AEF40F-FCD7-7D4B-B20B-948CAF16E68C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5325CC70-B9AA-AC49-8E12-5FCCD6C38B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31660" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="32000" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="238">
   <si>
     <t>Welcome</t>
   </si>
@@ -3492,7 +3492,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3681,7 +3681,9 @@
       <c r="B9" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="C9" s="80"/>
+      <c r="C9" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D9" s="81"/>
       <c r="E9" s="82"/>
       <c r="F9" s="81"/>
@@ -3697,7 +3699,9 @@
       <c r="A10" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="80"/>
+      <c r="B10" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="C10" s="80"/>
       <c r="D10" s="81"/>
       <c r="E10" s="82"/>
@@ -3707,7 +3711,7 @@
       <c r="I10" s="84"/>
       <c r="J10" s="85" t="str">
         <f t="shared" ref="J10:J17" si="2">IF(B10="","Waiting for spec","")</f>
-        <v>Waiting for spec</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" customHeight="1">
@@ -4040,7 +4044,9 @@
       <c r="A27" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="80"/>
+      <c r="B27" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="C27" s="80"/>
       <c r="D27" s="81"/>
       <c r="E27" s="82"/>
@@ -4050,7 +4056,7 @@
       <c r="I27" s="84"/>
       <c r="J27" s="85" t="str">
         <f t="shared" si="3"/>
-        <v>Waiting for spec</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1">
@@ -4135,11 +4141,11 @@
       </c>
       <c r="B32" s="68">
         <f t="shared" ref="B32:H32" si="5">COUNTIF(B3:B31, "&lt;&gt;")</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C32" s="68">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D32" s="65">
         <f t="shared" si="5"/>
@@ -4171,11 +4177,11 @@
       <c r="A33" s="71"/>
       <c r="B33" s="70">
         <f t="shared" ref="B33:H33" si="7">B32/$A32</f>
-        <v>0.82758620689655171</v>
+        <v>0.89655172413793105</v>
       </c>
       <c r="C33" s="70">
         <f t="shared" si="7"/>
-        <v>0.7931034482758621</v>
+        <v>0.82758620689655171</v>
       </c>
       <c r="D33" s="72">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Tightened up awards - especially sync and defaulted awards Removed sync from high scores dashboard from game summary Made sync OK for landscape
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5325CC70-B9AA-AC49-8E12-5FCCD6C38B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEAD473-3EB5-854B-A7AE-F4FF233DE68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32000" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="234">
   <si>
     <t>Welcome</t>
   </si>
@@ -783,18 +783,6 @@
   </si>
   <si>
     <t>Waiting for...</t>
-  </si>
-  <si>
-    <t>Check colors with Jack</t>
-  </si>
-  <si>
-    <t>Check with Jack</t>
-  </si>
-  <si>
-    <t>Check size with Jack</t>
-  </si>
-  <si>
-    <t>Shield definitions</t>
   </si>
 </sst>
 </file>
@@ -3492,7 +3480,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3561,8 +3549,12 @@
       <c r="C3" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="82"/>
+      <c r="D3" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F3" s="81"/>
       <c r="G3" s="82"/>
       <c r="H3" s="83"/>
@@ -3702,7 +3694,9 @@
       <c r="B10" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="C10" s="80"/>
+      <c r="C10" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D10" s="81"/>
       <c r="E10" s="82"/>
       <c r="F10" s="81"/>
@@ -3730,9 +3724,7 @@
       <c r="G11" s="82"/>
       <c r="H11" s="83"/>
       <c r="I11" s="84"/>
-      <c r="J11" s="85" t="s">
-        <v>236</v>
-      </c>
+      <c r="J11" s="85"/>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1">
       <c r="A12" s="79" t="s">
@@ -3744,8 +3736,12 @@
       <c r="C12" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="82"/>
+      <c r="D12" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E12" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F12" s="81"/>
       <c r="G12" s="82"/>
       <c r="H12" s="83"/>
@@ -3759,8 +3755,12 @@
       <c r="A13" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
+      <c r="B13" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>231</v>
+      </c>
       <c r="D13" s="81"/>
       <c r="E13" s="82"/>
       <c r="F13" s="81"/>
@@ -3769,7 +3769,7 @@
       <c r="I13" s="84"/>
       <c r="J13" s="85" t="str">
         <f t="shared" si="2"/>
-        <v>Waiting for spec</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" customHeight="1">
@@ -3788,9 +3788,7 @@
       <c r="G14" s="82"/>
       <c r="H14" s="83"/>
       <c r="I14" s="84"/>
-      <c r="J14" s="85" t="s">
-        <v>234</v>
-      </c>
+      <c r="J14" s="85"/>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1">
       <c r="A15" s="79" t="s">
@@ -3808,9 +3806,7 @@
       <c r="G15" s="82"/>
       <c r="H15" s="83"/>
       <c r="I15" s="84"/>
-      <c r="J15" s="85" t="s">
-        <v>235</v>
-      </c>
+      <c r="J15" s="85"/>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1">
       <c r="A16" s="79" t="s">
@@ -3864,15 +3860,17 @@
       <c r="C18" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D18" s="81"/>
-      <c r="E18" s="82"/>
+      <c r="D18" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F18" s="81"/>
       <c r="G18" s="82"/>
       <c r="H18" s="83"/>
       <c r="I18" s="84"/>
-      <c r="J18" s="85" t="s">
-        <v>237</v>
-      </c>
+      <c r="J18" s="85"/>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1">
       <c r="A19" s="79" t="s">
@@ -3884,8 +3882,12 @@
       <c r="C19" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D19" s="81"/>
-      <c r="E19" s="82"/>
+      <c r="D19" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F19" s="81"/>
       <c r="G19" s="82"/>
       <c r="H19" s="83"/>
@@ -3905,8 +3907,12 @@
       <c r="C20" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="82"/>
+      <c r="D20" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E20" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F20" s="81"/>
       <c r="G20" s="82"/>
       <c r="H20" s="83"/>
@@ -3926,8 +3932,12 @@
       <c r="C21" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="82"/>
+      <c r="D21" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F21" s="81"/>
       <c r="G21" s="82"/>
       <c r="H21" s="83"/>
@@ -3947,8 +3957,12 @@
       <c r="C22" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D22" s="81"/>
-      <c r="E22" s="82"/>
+      <c r="D22" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F22" s="81"/>
       <c r="G22" s="82"/>
       <c r="H22" s="83"/>
@@ -3968,15 +3982,17 @@
       <c r="C23" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="82"/>
+      <c r="D23" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E23" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F23" s="81"/>
       <c r="G23" s="82"/>
       <c r="H23" s="83"/>
       <c r="I23" s="84"/>
-      <c r="J23" s="85" t="s">
-        <v>235</v>
-      </c>
+      <c r="J23" s="85"/>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1">
       <c r="A24" s="79" t="s">
@@ -3988,8 +4004,12 @@
       <c r="C24" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="82"/>
+      <c r="D24" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E24" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F24" s="81"/>
       <c r="G24" s="82"/>
       <c r="H24" s="83"/>
@@ -4009,15 +4029,17 @@
       <c r="C25" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D25" s="81"/>
-      <c r="E25" s="82"/>
+      <c r="D25" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F25" s="81"/>
       <c r="G25" s="82"/>
       <c r="H25" s="83"/>
       <c r="I25" s="84"/>
-      <c r="J25" s="85" t="s">
-        <v>235</v>
-      </c>
+      <c r="J25" s="85"/>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1">
       <c r="A26" s="79" t="s">
@@ -4047,9 +4069,15 @@
       <c r="B27" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="C27" s="80"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
+      <c r="C27" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="D27" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E27" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F27" s="81"/>
       <c r="G27" s="82"/>
       <c r="H27" s="83"/>
@@ -4096,9 +4124,7 @@
       <c r="G29" s="82"/>
       <c r="H29" s="83"/>
       <c r="I29" s="84"/>
-      <c r="J29" s="85" t="s">
-        <v>235</v>
-      </c>
+      <c r="J29" s="85"/>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1">
       <c r="A30" s="79" t="s">
@@ -4141,19 +4167,19 @@
       </c>
       <c r="B32" s="68">
         <f t="shared" ref="B32:H32" si="5">COUNTIF(B3:B31, "&lt;&gt;")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C32" s="68">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D32" s="65">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E32" s="69">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F32" s="65">
         <f t="shared" si="5"/>
@@ -4177,19 +4203,19 @@
       <c r="A33" s="71"/>
       <c r="B33" s="70">
         <f t="shared" ref="B33:H33" si="7">B32/$A32</f>
-        <v>0.89655172413793105</v>
+        <v>0.93103448275862066</v>
       </c>
       <c r="C33" s="70">
         <f t="shared" si="7"/>
-        <v>0.82758620689655171</v>
+        <v>0.93103448275862066</v>
       </c>
       <c r="D33" s="72">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.37931034482758619</v>
       </c>
       <c r="E33" s="73">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.37931034482758619</v>
       </c>
       <c r="F33" s="72">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Sort out overrides in landscape and other minor changes
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEAD473-3EB5-854B-A7AE-F4FF233DE68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E1053E-37D9-4D4E-A2E8-AAA7AAF5B91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="235">
   <si>
     <t>Welcome</t>
   </si>
@@ -783,6 +783,9 @@
   </si>
   <si>
     <t>Waiting for...</t>
+  </si>
+  <si>
+    <t>?Yes</t>
   </si>
 </sst>
 </file>
@@ -3480,7 +3483,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="D29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3574,8 +3577,12 @@
       <c r="C4" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="82"/>
+      <c r="D4" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E4" s="82" t="s">
+        <v>234</v>
+      </c>
       <c r="F4" s="81"/>
       <c r="G4" s="82"/>
       <c r="H4" s="83"/>
@@ -3595,8 +3602,12 @@
       <c r="C5" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D5" s="81"/>
-      <c r="E5" s="82"/>
+      <c r="D5" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E5" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F5" s="81"/>
       <c r="G5" s="82"/>
       <c r="H5" s="83"/>
@@ -3616,8 +3627,12 @@
       <c r="C6" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
+      <c r="D6" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E6" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F6" s="81"/>
       <c r="G6" s="82"/>
       <c r="H6" s="83"/>
@@ -3637,8 +3652,12 @@
       <c r="C7" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="81"/>
-      <c r="E7" s="82"/>
+      <c r="D7" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F7" s="81"/>
       <c r="G7" s="82"/>
       <c r="H7" s="83"/>
@@ -3655,8 +3674,12 @@
       <c r="C8" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D8" s="81"/>
-      <c r="E8" s="82"/>
+      <c r="D8" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F8" s="81"/>
       <c r="G8" s="82"/>
       <c r="H8" s="83"/>
@@ -3676,8 +3699,12 @@
       <c r="C9" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="82"/>
+      <c r="D9" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E9" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F9" s="81"/>
       <c r="G9" s="82"/>
       <c r="H9" s="83"/>
@@ -3697,7 +3724,9 @@
       <c r="C10" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D10" s="81"/>
+      <c r="D10" s="81" t="s">
+        <v>231</v>
+      </c>
       <c r="E10" s="82"/>
       <c r="F10" s="81"/>
       <c r="G10" s="82"/>
@@ -3718,8 +3747,12 @@
       <c r="C11" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D11" s="81"/>
-      <c r="E11" s="82"/>
+      <c r="D11" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E11" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F11" s="81"/>
       <c r="G11" s="82"/>
       <c r="H11" s="83"/>
@@ -3818,8 +3851,12 @@
       <c r="C16" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D16" s="81"/>
-      <c r="E16" s="82"/>
+      <c r="D16" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E16" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F16" s="81"/>
       <c r="G16" s="82"/>
       <c r="H16" s="83"/>
@@ -3839,8 +3876,12 @@
       <c r="C17" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D17" s="81"/>
-      <c r="E17" s="82"/>
+      <c r="D17" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E17" s="82" t="s">
+        <v>234</v>
+      </c>
       <c r="F17" s="81"/>
       <c r="G17" s="82"/>
       <c r="H17" s="83"/>
@@ -4051,8 +4092,12 @@
       <c r="C26" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D26" s="81"/>
-      <c r="E26" s="82"/>
+      <c r="D26" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E26" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F26" s="81"/>
       <c r="G26" s="82"/>
       <c r="H26" s="83"/>
@@ -4118,8 +4163,12 @@
       <c r="C29" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="82"/>
+      <c r="D29" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" s="82" t="s">
+        <v>231</v>
+      </c>
       <c r="F29" s="81"/>
       <c r="G29" s="82"/>
       <c r="H29" s="83"/>
@@ -4175,11 +4224,11 @@
       </c>
       <c r="D32" s="65">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E32" s="69">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F32" s="65">
         <f t="shared" si="5"/>
@@ -4211,11 +4260,11 @@
       </c>
       <c r="D33" s="72">
         <f t="shared" si="7"/>
-        <v>0.37931034482758619</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="E33" s="73">
         <f t="shared" si="7"/>
-        <v>0.37931034482758619</v>
+        <v>0.75862068965517238</v>
       </c>
       <c r="F33" s="72">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Excluded computer players from sync Fixed bug where showing wrong player names under cards
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E1053E-37D9-4D4E-A2E8-AAA7AAF5B91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC958930-A321-D649-BF40-9835AD14A5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="225">
   <si>
     <t>Welcome</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Section Heading</t>
   </si>
   <si>
-    <t>Shape Fill</t>
-  </si>
-  <si>
     <t>Table Top</t>
   </si>
   <si>
@@ -177,12 +174,6 @@
     <t>Table top when playing</t>
   </si>
   <si>
-    <t>General welcome screen arrows</t>
-  </si>
-  <si>
-    <t>Highlighted welcome screen arrows</t>
-  </si>
-  <si>
     <t>Banner area of screen (and linked views)</t>
   </si>
   <si>
@@ -213,12 +204,6 @@
     <t>Banner / Logo</t>
   </si>
   <si>
-    <t>Other arrows</t>
-  </si>
-  <si>
-    <t>Game arrows</t>
-  </si>
-  <si>
     <t>Text on arrows</t>
   </si>
   <si>
@@ -349,15 +334,6 @@
   </si>
   <si>
     <t>Background / Text</t>
-  </si>
-  <si>
-    <t>Shape Stroke</t>
-  </si>
-  <si>
-    <t>Shape Highlight Fill</t>
-  </si>
-  <si>
-    <t>Shape Highlight Stroke</t>
   </si>
   <si>
     <t>Background of thumbnail when showing initials</t>
@@ -655,12 +631,6 @@
   </si>
   <si>
     <t>Use a 20% alpha if override button is disabled (no changes)</t>
-  </si>
-  <si>
-    <t>Shape Tabel Leg</t>
-  </si>
-  <si>
-    <t>Shape Table Leg Shadow</t>
   </si>
   <si>
     <t>Thumbnail placeholder</t>
@@ -913,7 +883,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -959,30 +929,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5B7B5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7B7B7B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED7674"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6F6F6F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCE736F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1054,18 +1000,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7BDAC7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF75CDBC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDCEEEA"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1369,7 +1303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1411,19 +1345,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1435,29 +1369,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1466,61 +1387,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1988,13 +1901,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
-  <dimension ref="A1:AD58"/>
+  <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:AD1"/>
+      <selection pane="bottomRight" activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2004,7 +1917,7 @@
     <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="11" width="21.6640625" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="50" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="42" customWidth="1"/>
     <col min="13" max="30" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2013,13 +1926,13 @@
         <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>0</v>
@@ -2042,7 +1955,7 @@
       <c r="K1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="41" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="12" t="s">
@@ -2058,16 +1971,16 @@
         <v>12</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="R1" s="12" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="U1" s="12" t="s">
         <v>14</v>
@@ -2105,10 +2018,10 @@
         <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -2117,25 +2030,25 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s">
         <v>24</v>
       </c>
       <c r="M2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="N2" t="s">
         <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="Q2" t="s">
         <v>24</v>
@@ -2144,10 +2057,10 @@
         <v>24</v>
       </c>
       <c r="S2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="T2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="U2" t="s">
         <v>24</v>
@@ -2175,32 +2088,32 @@
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>38</v>
+      <c r="B3" s="36" t="s">
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="O3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="Q3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="R3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="S3" t="s">
         <v>26</v>
@@ -2215,7 +2128,7 @@
         <v>26</v>
       </c>
       <c r="W3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="Y3" t="s">
         <v>26</v>
@@ -2224,19 +2137,19 @@
         <v>26</v>
       </c>
       <c r="AA3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AB3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4" s="44"/>
+        <v>193</v>
+      </c>
+      <c r="B4" s="36"/>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -2253,88 +2166,88 @@
         <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="O5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" s="45" t="s">
-        <v>38</v>
+        <v>190</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:30">
       <c r="A7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>38</v>
+        <v>195</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>37</v>
       </c>
       <c r="J7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" s="33" customFormat="1" ht="34">
-      <c r="A8" s="33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="28" customFormat="1" ht="34">
+      <c r="A8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="33" t="s">
+      <c r="B8" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="L8" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="O8" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="P8" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="V8" s="33" t="s">
-        <v>169</v>
+      <c r="K8" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="L8" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="P8" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="V8" s="28" t="s">
+        <v>161</v>
       </c>
       <c r="X8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" s="33" customFormat="1" ht="17">
-      <c r="A9" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="51"/>
-      <c r="U9" s="33" t="s">
-        <v>176</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" s="28" customFormat="1" ht="17">
+      <c r="A9" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="43"/>
+      <c r="U9" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="X9"/>
     </row>
@@ -2343,27 +2256,27 @@
         <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:30">
       <c r="A11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>38</v>
+        <v>196</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>37</v>
       </c>
       <c r="J11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -2371,76 +2284,76 @@
         <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J12" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>38</v>
+      <c r="B13" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="O13" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="35" t="s">
-        <v>178</v>
+      <c r="B14" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="O14" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="V14" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="AA14" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>181</v>
+        <v>172</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>173</v>
       </c>
       <c r="Y15" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="AA15" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -2448,27 +2361,27 @@
         <v>32</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:28">
       <c r="A17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>220</v>
+        <v>191</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>210</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="O17" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:28">
@@ -2476,584 +2389,837 @@
         <v>33</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N18" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="Q18" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="S18" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="T18" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="V18" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="Y18" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="AB18" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:28">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Y19" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="AB19" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:28">
       <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>178</v>
+        <v>34</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="J20" t="s">
         <v>26</v>
       </c>
       <c r="O20" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="P20" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:28">
       <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>38</v>
+        <v>86</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="R21" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:28">
       <c r="A22" t="s">
-        <v>199</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>38</v>
+        <v>189</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:28">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:28">
       <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" t="s">
+        <v>91</v>
+      </c>
+      <c r="M24" t="s">
+        <v>117</v>
+      </c>
+      <c r="O24" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>141</v>
+      </c>
+      <c r="S24" t="s">
+        <v>151</v>
+      </c>
+      <c r="T24" t="s">
+        <v>151</v>
+      </c>
+      <c r="U24" t="s">
+        <v>151</v>
+      </c>
+      <c r="V24" t="s">
+        <v>163</v>
+      </c>
+      <c r="W24" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:28">
       <c r="A25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>38</v>
+        <v>98</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" t="s">
+        <v>84</v>
+      </c>
+      <c r="U27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" t="s">
         <v>60</v>
       </c>
-      <c r="W25" s="1"/>
-    </row>
-    <row r="26" spans="1:28" s="25" customFormat="1">
-      <c r="A26" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L26" s="52"/>
-    </row>
-    <row r="27" spans="1:28" s="25" customFormat="1">
-      <c r="A27" s="25" t="s">
+      <c r="F28" t="s">
+        <v>60</v>
+      </c>
+      <c r="N28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>142</v>
+      </c>
+      <c r="U28" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
+      <c r="A29" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L27" s="52"/>
-    </row>
-    <row r="28" spans="1:28" s="25" customFormat="1">
-      <c r="A28" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="B28" s="40"/>
-      <c r="L28" s="52"/>
-    </row>
-    <row r="29" spans="1:28" s="25" customFormat="1">
-      <c r="A29" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="41"/>
-      <c r="L29" s="52"/>
+      <c r="B29" s="24"/>
+      <c r="C29" t="s">
+        <v>145</v>
+      </c>
+      <c r="I29" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="30" spans="1:28">
       <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>38</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B30" s="40"/>
       <c r="C30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="H30" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="J30" t="s">
-        <v>96</v>
-      </c>
-      <c r="M30" t="s">
-        <v>125</v>
+        <v>109</v>
+      </c>
+      <c r="N30" t="s">
+        <v>137</v>
       </c>
       <c r="O30" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="S30" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="T30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="U30" t="s">
-        <v>159</v>
-      </c>
-      <c r="V30" t="s">
-        <v>171</v>
-      </c>
-      <c r="W30" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="AA30" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AB30" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:28">
       <c r="A31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>38</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B31" s="15"/>
       <c r="C31" t="s">
-        <v>152</v>
+        <v>79</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="K31" t="s">
+        <v>111</v>
+      </c>
+      <c r="O31" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:28">
       <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>38</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B32" s="16"/>
       <c r="C32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>186</v>
+        <v>79</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+      <c r="K32" t="s">
+        <v>111</v>
+      </c>
+      <c r="O32" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:30">
       <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>38</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B33" s="17"/>
       <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="J33" t="s">
-        <v>89</v>
-      </c>
-      <c r="U33" t="s">
-        <v>167</v>
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K33" t="s">
+        <v>111</v>
+      </c>
+      <c r="O33" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:30">
       <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>38</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B34" s="26"/>
       <c r="C34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" t="s">
-        <v>65</v>
-      </c>
-      <c r="N34" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>150</v>
-      </c>
-      <c r="U34" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>185</v>
+        <v>146</v>
+      </c>
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+      <c r="O34" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:30">
       <c r="A35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="B35" s="25"/>
       <c r="C35" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" t="s">
-        <v>114</v>
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:30">
       <c r="A36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B36" s="48"/>
+        <v>76</v>
+      </c>
+      <c r="B36" s="18"/>
       <c r="C36" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" t="s">
-        <v>111</v>
-      </c>
-      <c r="J36" t="s">
-        <v>117</v>
-      </c>
-      <c r="N36" t="s">
-        <v>145</v>
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="K36" t="s">
+        <v>112</v>
       </c>
       <c r="O36" t="s">
-        <v>136</v>
-      </c>
-      <c r="S36" t="s">
-        <v>158</v>
-      </c>
-      <c r="T36" t="s">
-        <v>164</v>
-      </c>
-      <c r="U36" t="s">
-        <v>165</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>195</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:30">
       <c r="A37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="15"/>
+        <v>77</v>
+      </c>
+      <c r="B37" s="19"/>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K37" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="O37" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:30">
       <c r="A38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="16"/>
+        <v>75</v>
+      </c>
+      <c r="B38" s="17"/>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K38" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="O38" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30">
-      <c r="A39" t="s">
-        <v>83</v>
-      </c>
-      <c r="B39" s="17"/>
-      <c r="C39" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" t="s">
-        <v>86</v>
-      </c>
-      <c r="K39" t="s">
-        <v>119</v>
-      </c>
-      <c r="O39" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30">
-      <c r="A40" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="31"/>
-      <c r="C40" t="s">
-        <v>154</v>
-      </c>
-      <c r="D40" t="s">
-        <v>128</v>
-      </c>
-      <c r="O40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" s="20" customFormat="1" ht="51">
+      <c r="A39" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="21"/>
+      <c r="J39" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="L39" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="N39" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="O39" s="20" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="41" spans="1:30">
-      <c r="A41" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="30"/>
-      <c r="C41" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" t="s">
-        <v>129</v>
+      <c r="R39" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="U39" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="V39" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z39" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB39" s="20" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:30">
       <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="18"/>
-      <c r="C42" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" t="s">
-        <v>87</v>
-      </c>
-      <c r="K42" t="s">
-        <v>120</v>
-      </c>
-      <c r="O42" t="s">
-        <v>141</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L42" s="45"/>
+      <c r="M42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
     </row>
     <row r="43" spans="1:30">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="19"/>
-      <c r="C43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-      <c r="K43" t="s">
-        <v>120</v>
-      </c>
-      <c r="O43" t="s">
-        <v>141</v>
-      </c>
+      <c r="B43" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L43" s="45"/>
+      <c r="M43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="1:30">
       <c r="A44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="17"/>
-      <c r="C44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" t="s">
-        <v>87</v>
-      </c>
-      <c r="K44" t="s">
-        <v>120</v>
-      </c>
-      <c r="O44" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:30" s="20" customFormat="1" ht="51">
-      <c r="A45" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="21"/>
-      <c r="J45" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="L45" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="N45" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="O45" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="R45" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="U45" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="V45" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z45" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="AB45" s="20" t="s">
-        <v>196</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L44" s="45"/>
+      <c r="M44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="P44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3"/>
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="3"/>
+    </row>
+    <row r="45" spans="1:30">
+      <c r="B45" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L45" s="45"/>
+      <c r="M45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="3"/>
+      <c r="AC45" s="3"/>
+      <c r="AD45" s="3"/>
+    </row>
+    <row r="46" spans="1:30">
+      <c r="A46" t="s">
+        <v>201</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L46" s="45"/>
+      <c r="M46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="P46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3"/>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3"/>
+      <c r="AC46" s="3"/>
+      <c r="AD46" s="3"/>
+    </row>
+    <row r="47" spans="1:30">
+      <c r="B47" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L47" s="45"/>
+      <c r="M47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="P47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
+      <c r="X47" s="3"/>
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="3"/>
+      <c r="AA47" s="3"/>
+      <c r="AB47" s="3"/>
+      <c r="AC47" s="3"/>
+      <c r="AD47" s="3"/>
     </row>
     <row r="48" spans="1:30">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>209</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L48" s="54"/>
+        <v>203</v>
+      </c>
+      <c r="L48" s="45"/>
       <c r="M48" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="N48" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q48" s="3" t="s">
-        <v>213</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
@@ -3068,47 +3234,46 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
     </row>
-    <row r="49" spans="1:30">
+    <row r="49" spans="2:30">
       <c r="B49" s="3" t="s">
-        <v>208</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L49" s="54"/>
+        <v>203</v>
+      </c>
+      <c r="L49" s="45"/>
       <c r="M49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q49" s="3" t="s">
-        <v>213</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
@@ -3123,352 +3288,27 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
     </row>
-    <row r="50" spans="1:30">
-      <c r="A50" t="s">
-        <v>210</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L50" s="54"/>
-      <c r="M50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="N50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="O50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-      <c r="V50" s="3"/>
-      <c r="W50" s="3"/>
-      <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
-      <c r="AA50" s="3"/>
-      <c r="AB50" s="3"/>
-      <c r="AC50" s="3"/>
-      <c r="AD50" s="3"/>
-    </row>
-    <row r="51" spans="1:30">
-      <c r="B51" s="3" t="s">
+    <row r="50" spans="2:30">
+      <c r="G50" t="s">
+        <v>205</v>
+      </c>
+      <c r="H50" t="s">
         <v>208</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L51" s="54"/>
-      <c r="M51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="N51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="O51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
-      <c r="AA51" s="3"/>
-      <c r="AB51" s="3"/>
-      <c r="AC51" s="3"/>
-      <c r="AD51" s="3"/>
-    </row>
-    <row r="52" spans="1:30">
-      <c r="A52" t="s">
-        <v>211</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L52" s="54"/>
-      <c r="M52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="N52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="O52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P52" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
-      <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
-      <c r="Z52" s="3"/>
-      <c r="AA52" s="3"/>
-      <c r="AB52" s="3"/>
-      <c r="AC52" s="3"/>
-      <c r="AD52" s="3"/>
-    </row>
-    <row r="53" spans="1:30">
-      <c r="B53" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L53" s="54"/>
-      <c r="M53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="N53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="O53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P53" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-      <c r="S53" s="3"/>
-      <c r="T53" s="3"/>
-      <c r="U53" s="3"/>
-      <c r="V53" s="3"/>
-      <c r="W53" s="3"/>
-      <c r="X53" s="3"/>
-      <c r="Y53" s="3"/>
-      <c r="Z53" s="3"/>
-      <c r="AA53" s="3"/>
-      <c r="AB53" s="3"/>
-      <c r="AC53" s="3"/>
-      <c r="AD53" s="3"/>
-    </row>
-    <row r="54" spans="1:30">
-      <c r="A54" t="s">
-        <v>212</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L54" s="54"/>
-      <c r="M54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="N54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="O54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P54" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q54" s="3"/>
-      <c r="R54" s="3"/>
-      <c r="S54" s="3"/>
-      <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-      <c r="V54" s="3"/>
-      <c r="W54" s="3"/>
-      <c r="X54" s="3"/>
-      <c r="Y54" s="3"/>
-      <c r="Z54" s="3"/>
-      <c r="AA54" s="3"/>
-      <c r="AB54" s="3"/>
-      <c r="AC54" s="3"/>
-      <c r="AD54" s="3"/>
-    </row>
-    <row r="55" spans="1:30">
-      <c r="B55" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L55" s="54"/>
-      <c r="M55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="N55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="O55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P55" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
-      <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
-      <c r="Z55" s="3"/>
-      <c r="AA55" s="3"/>
-      <c r="AB55" s="3"/>
-      <c r="AC55" s="3"/>
-      <c r="AD55" s="3"/>
-    </row>
-    <row r="56" spans="1:30">
-      <c r="G56" t="s">
-        <v>215</v>
-      </c>
-      <c r="H56" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="57" spans="1:30">
-      <c r="G57" t="s">
-        <v>216</v>
-      </c>
-      <c r="H57" t="s">
+    </row>
+    <row r="51" spans="2:30">
+      <c r="G51" t="s">
+        <v>206</v>
+      </c>
+      <c r="H51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:30">
-      <c r="G58" t="s">
-        <v>217</v>
-      </c>
-      <c r="H58" t="s">
+    <row r="52" spans="2:30">
+      <c r="G52" t="s">
+        <v>207</v>
+      </c>
+      <c r="H52" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3482,807 +3322,807 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD168BF6-7604-814B-8525-59664C788955}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="55" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" style="46" customWidth="1"/>
     <col min="10" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1">
-      <c r="A1" s="59"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="92" t="s">
-        <v>228</v>
-      </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="94" t="s">
+      <c r="A1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="83" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="84"/>
+      <c r="F1" s="83" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="84"/>
+      <c r="H1" s="85" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="86"/>
+      <c r="J1" s="66"/>
+    </row>
+    <row r="2" spans="1:10" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A2" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="J2" s="67" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16" customHeight="1">
+      <c r="A3" s="70" t="s">
         <v>212</v>
       </c>
-      <c r="I1" s="95"/>
-      <c r="J1" s="75"/>
-    </row>
-    <row r="2" spans="1:10" s="56" customFormat="1" ht="16" customHeight="1" thickBot="1">
-      <c r="A2" s="60" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>232</v>
-      </c>
-      <c r="C2" s="62" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" s="63" t="s">
-        <v>229</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>230</v>
-      </c>
-      <c r="H2" s="57" t="s">
-        <v>229</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="J2" s="76" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16" customHeight="1">
-      <c r="A3" s="79" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C3" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D3" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85" t="str">
+      <c r="B3" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="76" t="str">
         <f t="shared" ref="J3:J6" si="0">IF(B3="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" customHeight="1">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C4" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D4" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E4" s="82" t="s">
-        <v>234</v>
-      </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="85" t="str">
+      <c r="B4" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" s="72"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16" customHeight="1">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C5" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D5" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E5" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85" t="str">
+      <c r="B5" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="72"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16" customHeight="1">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C6" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D6" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E6" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F6" s="81"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="85" t="str">
+      <c r="B6" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="72"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16" customHeight="1">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C7" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D7" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E7" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="85"/>
+      <c r="B7" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" s="72"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="76"/>
     </row>
     <row r="8" spans="1:10" ht="16" customHeight="1">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C8" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D8" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E8" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F8" s="81"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="85" t="str">
+      <c r="B8" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="72"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="76" t="str">
         <f t="shared" ref="J8:J9" si="1">IF(B8="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16" customHeight="1">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D9" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E9" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" s="81"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85" t="str">
+      <c r="B9" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E9" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="72"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="76" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16" customHeight="1">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D10" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="85" t="str">
+      <c r="B10" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="73"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="76" t="str">
         <f t="shared" ref="J10:J17" si="2">IF(B10="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" customHeight="1">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C11" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D11" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E11" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="85"/>
+      <c r="B11" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" s="72"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C12" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E12" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F12" s="81"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="85" t="str">
+      <c r="B12" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F12" s="72"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16" customHeight="1">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C13" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D13" s="81"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="85" t="str">
+      <c r="B13" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D13" s="72"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" customHeight="1">
-      <c r="A14" s="79" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C14" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="85"/>
+      <c r="A14" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14" s="72"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="76"/>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C15" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="85"/>
+      <c r="B15" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="72"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="76"/>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1">
-      <c r="A16" s="79" t="s">
-        <v>224</v>
-      </c>
-      <c r="B16" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C16" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D16" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E16" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F16" s="81"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="85" t="str">
+      <c r="A16" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F16" s="72"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" customHeight="1">
-      <c r="A17" s="79" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C17" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D17" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>234</v>
-      </c>
-      <c r="F17" s="81"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="85" t="str">
+      <c r="A17" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="F17" s="72"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:10" ht="17">
-      <c r="A18" s="79" t="s">
-        <v>225</v>
-      </c>
-      <c r="B18" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C18" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D18" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E18" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F18" s="81"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="85"/>
+      <c r="A18" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E18" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F18" s="72"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="76"/>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C19" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D19" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E19" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F19" s="81"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="85" t="str">
+      <c r="B19" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" s="72"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="76" t="str">
         <f t="shared" ref="J19:J31" si="3">IF(B19="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16" customHeight="1">
-      <c r="A20" s="79" t="s">
-        <v>162</v>
-      </c>
-      <c r="B20" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C20" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D20" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E20" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F20" s="81"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="85" t="str">
+      <c r="A20" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" s="72"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="76" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16" customHeight="1">
-      <c r="A21" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="B21" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C21" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D21" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E21" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F21" s="81"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="85" t="str">
+      <c r="A21" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E21" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="72"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="76" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C22" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D22" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E22" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F22" s="81"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="85" t="str">
+      <c r="B22" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F22" s="72"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="76" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C23" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D23" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E23" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F23" s="81"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="85"/>
+      <c r="B23" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D23" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F23" s="72"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="76"/>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1">
-      <c r="A24" s="79" t="s">
+      <c r="A24" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C24" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D24" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E24" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F24" s="81"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="85" t="str">
+      <c r="B24" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E24" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="72"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="76" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C25" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D25" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E25" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F25" s="81"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="85"/>
+      <c r="B25" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E25" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="72"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="76"/>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C26" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D26" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E26" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F26" s="81"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="85" t="str">
+      <c r="B26" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D26" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E26" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F26" s="72"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="76" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C27" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D27" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E27" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F27" s="81"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="85" t="str">
+      <c r="B27" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D27" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E27" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F27" s="72"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="76" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C28" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D28" s="81"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="85" t="str">
+      <c r="B28" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D28" s="72"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="76" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="C29" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D29" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E29" s="82" t="s">
-        <v>231</v>
-      </c>
-      <c r="F29" s="81"/>
-      <c r="G29" s="82"/>
-      <c r="H29" s="83"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="85"/>
+      <c r="B29" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D29" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F29" s="72"/>
+      <c r="G29" s="73"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="76"/>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="84"/>
-      <c r="J30" s="85" t="str">
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="76" t="str">
         <f t="shared" si="3"/>
         <v>Waiting for spec</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1" thickBot="1">
-      <c r="A31" s="86" t="s">
+      <c r="A31" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="85" t="str">
+      <c r="B31" s="78"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="76" t="str">
         <f t="shared" si="3"/>
         <v>Waiting for spec</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="17" thickBot="1">
-      <c r="A32" s="67">
+      <c r="A32" s="58">
         <f t="shared" ref="A32" si="4">COUNTIF(A3:A31, "&lt;&gt;")</f>
         <v>29</v>
       </c>
-      <c r="B32" s="68">
+      <c r="B32" s="59">
         <f t="shared" ref="B32:H32" si="5">COUNTIF(B3:B31, "&lt;&gt;")</f>
         <v>27</v>
       </c>
-      <c r="C32" s="68">
+      <c r="C32" s="59">
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="D32" s="65">
+      <c r="D32" s="56">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="E32" s="69">
+      <c r="E32" s="60">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="F32" s="65">
+      <c r="F32" s="56">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G32" s="69">
+      <c r="G32" s="60">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H32" s="65">
+      <c r="H32" s="56">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I32" s="66">
+      <c r="I32" s="57">
         <f t="shared" ref="I32" si="6">COUNTIF(I3:I31, "&lt;&gt;")</f>
         <v>0</v>
       </c>
-      <c r="J32" s="77"/>
+      <c r="J32" s="68"/>
     </row>
     <row r="33" spans="1:10" ht="17" thickBot="1">
-      <c r="A33" s="71"/>
-      <c r="B33" s="70">
+      <c r="A33" s="62"/>
+      <c r="B33" s="61">
         <f t="shared" ref="B33:H33" si="7">B32/$A32</f>
         <v>0.93103448275862066</v>
       </c>
-      <c r="C33" s="70">
+      <c r="C33" s="61">
         <f t="shared" si="7"/>
         <v>0.93103448275862066</v>
       </c>
-      <c r="D33" s="72">
+      <c r="D33" s="63">
         <f t="shared" si="7"/>
         <v>0.7931034482758621</v>
       </c>
-      <c r="E33" s="73">
+      <c r="E33" s="64">
         <f t="shared" si="7"/>
         <v>0.75862068965517238</v>
       </c>
-      <c r="F33" s="72">
+      <c r="F33" s="63">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G33" s="73">
+      <c r="G33" s="64">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H33" s="72">
+      <c r="H33" s="63">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I33" s="74">
+      <c r="I33" s="65">
         <f t="shared" ref="I33" si="8">I32/$A32</f>
         <v>0</v>
       </c>
-      <c r="J33" s="78"/>
+      <c r="J33" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
First new UI for iPad
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC958930-A321-D649-BF40-9835AD14A5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E81EC69-4278-DD41-937B-BFCBEF8B1D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView minimized="1" xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="228">
   <si>
     <t>Welcome</t>
   </si>
@@ -756,6 +756,15 @@
   </si>
   <si>
     <t>?Yes</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E206-C2AF-6148-A40D-84341520B72E}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3320,10 +3329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD168BF6-7604-814B-8525-59664C788955}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3332,7 +3341,7 @@
     <col min="10" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="50"/>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -3350,7 +3359,7 @@
       <c r="I1" s="86"/>
       <c r="J1" s="66"/>
     </row>
-    <row r="2" spans="1:10" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="2" spans="1:11" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="51" t="s">
         <v>211</v>
       </c>
@@ -3382,7 +3391,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" customHeight="1">
+    <row r="3" spans="1:11" ht="16" customHeight="1">
       <c r="A3" s="70" t="s">
         <v>212</v>
       </c>
@@ -3407,7 +3416,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" customHeight="1">
+    <row r="4" spans="1:11" ht="16" customHeight="1">
       <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
@@ -3431,8 +3440,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="16" customHeight="1">
+      <c r="K4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" customHeight="1">
       <c r="A5" s="70" t="s">
         <v>2</v>
       </c>
@@ -3456,8 +3468,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="16" customHeight="1">
+      <c r="K5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16" customHeight="1">
       <c r="A6" s="70" t="s">
         <v>3</v>
       </c>
@@ -3481,8 +3496,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="16" customHeight="1">
+      <c r="K6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" customHeight="1">
       <c r="A7" s="70" t="s">
         <v>4</v>
       </c>
@@ -3503,8 +3521,11 @@
       <c r="H7" s="74"/>
       <c r="I7" s="75"/>
       <c r="J7" s="76"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" customHeight="1">
+      <c r="K7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" customHeight="1">
       <c r="A8" s="70" t="s">
         <v>5</v>
       </c>
@@ -3528,8 +3549,11 @@
         <f t="shared" ref="J8:J9" si="1">IF(B8="","Waiting for spec","")</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="16" customHeight="1">
+      <c r="K8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" customHeight="1">
       <c r="A9" s="70" t="s">
         <v>6</v>
       </c>
@@ -3553,8 +3577,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="16" customHeight="1">
+      <c r="K9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" customHeight="1">
       <c r="A10" s="70" t="s">
         <v>7</v>
       </c>
@@ -3576,8 +3603,11 @@
         <f t="shared" ref="J10:J17" si="2">IF(B10="","Waiting for spec","")</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="16" customHeight="1">
+      <c r="K10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" customHeight="1">
       <c r="A11" s="70" t="s">
         <v>8</v>
       </c>
@@ -3598,8 +3628,11 @@
       <c r="H11" s="74"/>
       <c r="I11" s="75"/>
       <c r="J11" s="76"/>
-    </row>
-    <row r="12" spans="1:10" ht="16" customHeight="1">
+      <c r="K11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" customHeight="1">
       <c r="A12" s="70" t="s">
         <v>10</v>
       </c>
@@ -3623,8 +3656,11 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="16" customHeight="1">
+      <c r="K12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16" customHeight="1">
       <c r="A13" s="70" t="s">
         <v>11</v>
       </c>
@@ -3644,8 +3680,11 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="16" customHeight="1">
+      <c r="K13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16" customHeight="1">
       <c r="A14" s="70" t="s">
         <v>213</v>
       </c>
@@ -3662,8 +3701,11 @@
       <c r="H14" s="74"/>
       <c r="I14" s="75"/>
       <c r="J14" s="76"/>
-    </row>
-    <row r="15" spans="1:10" ht="16" customHeight="1">
+      <c r="K14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" customHeight="1">
       <c r="A15" s="70" t="s">
         <v>12</v>
       </c>
@@ -3680,8 +3722,11 @@
       <c r="H15" s="74"/>
       <c r="I15" s="75"/>
       <c r="J15" s="76"/>
-    </row>
-    <row r="16" spans="1:10" ht="16" customHeight="1">
+      <c r="K15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" customHeight="1">
       <c r="A16" s="70" t="s">
         <v>214</v>
       </c>
@@ -3705,8 +3750,11 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="16" customHeight="1">
+      <c r="K16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16" customHeight="1">
       <c r="A17" s="70" t="s">
         <v>122</v>
       </c>
@@ -3730,8 +3778,11 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="17">
+      <c r="K17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17">
       <c r="A18" s="70" t="s">
         <v>215</v>
       </c>
@@ -3752,8 +3803,11 @@
       <c r="H18" s="74"/>
       <c r="I18" s="75"/>
       <c r="J18" s="76"/>
-    </row>
-    <row r="19" spans="1:10" ht="16" customHeight="1">
+      <c r="K18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16" customHeight="1">
       <c r="A19" s="70" t="s">
         <v>13</v>
       </c>
@@ -3774,11 +3828,14 @@
       <c r="H19" s="74"/>
       <c r="I19" s="75"/>
       <c r="J19" s="76" t="str">
-        <f t="shared" ref="J19:J31" si="3">IF(B19="","Waiting for spec","")</f>
+        <f t="shared" ref="J19:K31" si="3">IF(B19="","Waiting for spec","")</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="16" customHeight="1">
+      <c r="K19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" customHeight="1">
       <c r="A20" s="70" t="s">
         <v>154</v>
       </c>
@@ -3802,8 +3859,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="16" customHeight="1">
+      <c r="K20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" customHeight="1">
       <c r="A21" s="70" t="s">
         <v>155</v>
       </c>
@@ -3827,8 +3887,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="16" customHeight="1">
+      <c r="K21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" customHeight="1">
       <c r="A22" s="70" t="s">
         <v>14</v>
       </c>
@@ -3852,8 +3915,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="16" customHeight="1">
+      <c r="K22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16" customHeight="1">
       <c r="A23" s="70" t="s">
         <v>15</v>
       </c>
@@ -3874,8 +3940,11 @@
       <c r="H23" s="74"/>
       <c r="I23" s="75"/>
       <c r="J23" s="76"/>
-    </row>
-    <row r="24" spans="1:10" ht="16" customHeight="1">
+      <c r="K23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" customHeight="1">
       <c r="A24" s="70" t="s">
         <v>16</v>
       </c>
@@ -3899,8 +3968,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="16" customHeight="1">
+      <c r="K24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16" customHeight="1">
       <c r="A25" s="70" t="s">
         <v>17</v>
       </c>
@@ -3921,8 +3993,11 @@
       <c r="H25" s="74"/>
       <c r="I25" s="75"/>
       <c r="J25" s="76"/>
-    </row>
-    <row r="26" spans="1:10" ht="16" customHeight="1">
+      <c r="K25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16" customHeight="1">
       <c r="A26" s="70" t="s">
         <v>18</v>
       </c>
@@ -3946,8 +4021,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="16" customHeight="1">
+      <c r="K26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16" customHeight="1">
       <c r="A27" s="70" t="s">
         <v>19</v>
       </c>
@@ -3971,8 +4049,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="16" customHeight="1">
+      <c r="K27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" customHeight="1">
       <c r="A28" s="70" t="s">
         <v>20</v>
       </c>
@@ -3992,8 +4073,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="16" customHeight="1">
+      <c r="K28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" customHeight="1">
       <c r="A29" s="70" t="s">
         <v>21</v>
       </c>
@@ -4014,8 +4098,11 @@
       <c r="H29" s="74"/>
       <c r="I29" s="75"/>
       <c r="J29" s="76"/>
-    </row>
-    <row r="30" spans="1:10" ht="16" customHeight="1">
+      <c r="K29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" customHeight="1">
       <c r="A30" s="70" t="s">
         <v>22</v>
       </c>
@@ -4031,8 +4118,12 @@
         <f t="shared" si="3"/>
         <v>Waiting for spec</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="16" customHeight="1" thickBot="1">
+      <c r="K30" s="76" t="str">
+        <f t="shared" si="3"/>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16" customHeight="1" thickBot="1">
       <c r="A31" s="77" t="s">
         <v>23</v>
       </c>
@@ -4049,7 +4140,7 @@
         <v>Waiting for spec</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17" thickBot="1">
+    <row r="32" spans="1:11" ht="17" thickBot="1">
       <c r="A32" s="58">
         <f t="shared" ref="A32" si="4">COUNTIF(A3:A31, "&lt;&gt;")</f>
         <v>29</v>
@@ -4135,7 +4226,7 @@
       <formula>AND($B3="Yes", $C3="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19:J31">
+  <conditionalFormatting sqref="J19:J31 K30">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($B19="Yes", $C19="")</formula>
     </cfRule>

</xml_diff>

<commit_message>
Copy before attach game view controllers
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E81EC69-4278-DD41-937B-BFCBEF8B1D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058A6E37-FC58-C649-B252-BAAC3696A5E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="226">
   <si>
     <t>Welcome</t>
   </si>
@@ -758,13 +758,7 @@
     <t>?Yes</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1560,6 +1554,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3329,35 +3324,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD168BF6-7604-814B-8525-59664C788955}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.1640625" style="46" customWidth="1"/>
-    <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="50"/>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="87"/>
+      <c r="E1" s="83" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="84"/>
+      <c r="G1" s="83" t="s">
         <v>218</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="85" t="s">
+      <c r="H1" s="84"/>
+      <c r="I1" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="66"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:11" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="51" t="s">
@@ -3369,25 +3365,28 @@
       <c r="C2" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="F2" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="G2" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="H2" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="I2" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="J2" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="J2" s="67" t="s">
+      <c r="K2" s="67" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3401,18 +3400,21 @@
       <c r="C3" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D3" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E3" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76" t="str">
-        <f t="shared" ref="J3:J6" si="0">IF(B3="","Waiting for spec","")</f>
+      <c r="D3" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3" s="72"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="76" t="str">
+        <f t="shared" ref="K3:K6" si="0">IF(B3="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
@@ -3426,22 +3428,22 @@
       <c r="C4" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" s="73" t="s">
+      <c r="D4" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="76" t="str">
+      <c r="G4" s="72"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="K4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16" customHeight="1">
@@ -3454,22 +3456,22 @@
       <c r="C5" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E5" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="76" t="str">
+      <c r="D5" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="K5" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16" customHeight="1">
@@ -3482,22 +3484,22 @@
       <c r="C6" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E6" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F6" s="72"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="76" t="str">
+      <c r="D6" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G6" s="72"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="K6" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16" customHeight="1">
@@ -3510,20 +3512,18 @@
       <c r="C7" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D7" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E7" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F7" s="72"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
-      <c r="K7" t="s">
-        <v>225</v>
-      </c>
+      <c r="D7" s="74"/>
+      <c r="E7" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="76"/>
     </row>
     <row r="8" spans="1:11" ht="16" customHeight="1">
       <c r="A8" s="70" t="s">
@@ -3535,22 +3535,20 @@
       <c r="C8" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D8" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E8" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F8" s="72"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="76" t="str">
-        <f t="shared" ref="J8:J9" si="1">IF(B8="","Waiting for spec","")</f>
+      <c r="D8" s="74"/>
+      <c r="E8" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="76" t="str">
+        <f t="shared" ref="K8:K9" si="1">IF(B8="","Waiting for spec","")</f>
         <v/>
-      </c>
-      <c r="K8" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16" customHeight="1">
@@ -3563,22 +3561,20 @@
       <c r="C9" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D9" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E9" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F9" s="72"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="76" t="str">
+      <c r="D9" s="74"/>
+      <c r="E9" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G9" s="72"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="76" t="str">
         <f t="shared" si="1"/>
         <v/>
-      </c>
-      <c r="K9" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16" customHeight="1">
@@ -3591,20 +3587,18 @@
       <c r="C10" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D10" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="76" t="str">
-        <f t="shared" ref="J10:J17" si="2">IF(B10="","Waiting for spec","")</f>
+      <c r="D10" s="74"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" s="72"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="76" t="str">
+        <f t="shared" ref="K10:K17" si="2">IF(B10="","Waiting for spec","")</f>
         <v/>
-      </c>
-      <c r="K10" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16" customHeight="1">
@@ -3617,20 +3611,20 @@
       <c r="C11" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D11" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E11" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F11" s="72"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="76"/>
-      <c r="K11" t="s">
-        <v>227</v>
-      </c>
+      <c r="D11" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G11" s="72"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
     </row>
     <row r="12" spans="1:11" ht="16" customHeight="1">
       <c r="A12" s="70" t="s">
@@ -3642,22 +3636,22 @@
       <c r="C12" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D12" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E12" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F12" s="72"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="76" t="str">
+      <c r="D12" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F12" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G12" s="72"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
-      </c>
-      <c r="K12" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16" customHeight="1">
@@ -3670,18 +3664,20 @@
       <c r="C13" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="76" t="str">
+      <c r="D13" s="74"/>
+      <c r="E13" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F13" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G13" s="72"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
-      </c>
-      <c r="K13" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16" customHeight="1">
@@ -3694,16 +3690,20 @@
       <c r="C14" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="76"/>
-      <c r="K14" t="s">
-        <v>203</v>
-      </c>
+      <c r="D14" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G14" s="72"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="76"/>
     </row>
     <row r="15" spans="1:11" ht="16" customHeight="1">
       <c r="A15" s="70" t="s">
@@ -3715,16 +3715,18 @@
       <c r="C15" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="76"/>
-      <c r="K15" t="s">
-        <v>225</v>
-      </c>
+      <c r="D15" s="74"/>
+      <c r="E15" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G15" s="72"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="76"/>
     </row>
     <row r="16" spans="1:11" ht="16" customHeight="1">
       <c r="A16" s="70" t="s">
@@ -3736,25 +3738,25 @@
       <c r="C16" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D16" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E16" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F16" s="72"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="76" t="str">
+      <c r="D16" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G16" s="72"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="16" customHeight="1">
+    </row>
+    <row r="17" spans="1:12" ht="16" customHeight="1">
       <c r="A17" s="70" t="s">
         <v>122</v>
       </c>
@@ -3764,25 +3766,25 @@
       <c r="C17" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D17" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E17" s="73" t="s">
+      <c r="D17" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F17" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="F17" s="72"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="76" t="str">
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K17" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="17">
+    </row>
+    <row r="18" spans="1:12" ht="17">
       <c r="A18" s="70" t="s">
         <v>215</v>
       </c>
@@ -3792,22 +3794,22 @@
       <c r="C18" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D18" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F18" s="72"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="76"/>
-      <c r="K18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="16" customHeight="1">
+      <c r="D18" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G18" s="72"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="76"/>
+    </row>
+    <row r="19" spans="1:12" ht="16" customHeight="1">
       <c r="A19" s="70" t="s">
         <v>13</v>
       </c>
@@ -3817,25 +3819,25 @@
       <c r="C19" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E19" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F19" s="72"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="76" t="str">
-        <f t="shared" ref="J19:K31" si="3">IF(B19="","Waiting for spec","")</f>
+      <c r="D19" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="76" t="str">
+        <f>IF(B19="","Waiting for spec","")</f>
         <v/>
       </c>
-      <c r="K19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="16" customHeight="1">
+    </row>
+    <row r="20" spans="1:12" ht="16" customHeight="1">
       <c r="A20" s="70" t="s">
         <v>154</v>
       </c>
@@ -3845,25 +3847,23 @@
       <c r="C20" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D20" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E20" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F20" s="72"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G20" s="72"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="76" t="str">
+        <f>IF(B20="","Waiting for spec","")</f>
         <v/>
       </c>
-      <c r="K20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="16" customHeight="1">
+    </row>
+    <row r="21" spans="1:12" ht="16" customHeight="1">
       <c r="A21" s="70" t="s">
         <v>155</v>
       </c>
@@ -3873,25 +3873,23 @@
       <c r="C21" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E21" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F21" s="72"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G21" s="72"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="76" t="str">
+        <f>IF(B21="","Waiting for spec","")</f>
         <v/>
       </c>
-      <c r="K21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="16" customHeight="1">
+    </row>
+    <row r="22" spans="1:12" ht="16" customHeight="1">
       <c r="A22" s="70" t="s">
         <v>14</v>
       </c>
@@ -3901,25 +3899,23 @@
       <c r="C22" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D22" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E22" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F22" s="72"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F22" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G22" s="72"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="76" t="str">
+        <f>IF(B22="","Waiting for spec","")</f>
         <v/>
       </c>
-      <c r="K22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="16" customHeight="1">
+    </row>
+    <row r="23" spans="1:12" ht="16" customHeight="1">
       <c r="A23" s="70" t="s">
         <v>15</v>
       </c>
@@ -3929,24 +3925,22 @@
       <c r="C23" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D23" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E23" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F23" s="72"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="76"/>
-      <c r="K23" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="16" customHeight="1">
+      <c r="D23" s="74"/>
+      <c r="E23" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F23" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="76"/>
+    </row>
+    <row r="24" spans="1:12" ht="16" customHeight="1">
       <c r="A24" s="70" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B24" s="71" t="s">
         <v>221</v>
@@ -3954,281 +3948,262 @@
       <c r="C24" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E24" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F24" s="72"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="76" t="str">
+      <c r="D24" s="74"/>
+      <c r="E24" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G24" s="72"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="76"/>
+    </row>
+    <row r="25" spans="1:12" ht="16" customHeight="1">
+      <c r="A25" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E25" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" s="72"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="76" t="str">
+        <f>IF(B25="","Waiting for spec","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="16" customHeight="1">
+      <c r="A26" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D26" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F26" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G26" s="72"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="76" t="str">
+        <f>IF(B26="","Waiting for spec","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="16" customHeight="1">
+      <c r="A27" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D27" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E27" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F27" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G27" s="72"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="76" t="str">
+        <f>IF(B27="","Waiting for spec","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16" customHeight="1">
+      <c r="A28" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D28" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="F28" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="G28" s="72"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="76"/>
+    </row>
+    <row r="29" spans="1:12" ht="16" customHeight="1">
+      <c r="A29" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="76" t="str">
+        <f>IF(B29="","Waiting for spec","")</f>
+        <v>Waiting for spec</v>
+      </c>
+      <c r="L29" s="76"/>
+    </row>
+    <row r="30" spans="1:12" ht="16" customHeight="1" thickBot="1">
+      <c r="A30" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="76" t="str">
+        <f>IF(B30="","Waiting for spec","")</f>
+        <v>Waiting for spec</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="17" thickBot="1">
+      <c r="A31" s="58">
+        <f>COUNTIF(A3:A30, "&lt;&gt;")</f>
+        <v>28</v>
+      </c>
+      <c r="B31" s="59">
+        <f>COUNTIF(B3:B30, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+      <c r="C31" s="59">
+        <f>COUNTIF(C3:C30, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+      <c r="D31" s="59">
+        <f>COUNTIF(D3:D30, "&lt;&gt;")</f>
+        <v>15</v>
+      </c>
+      <c r="E31" s="56">
+        <f>COUNTIF(E3:E30, "&lt;&gt;")</f>
+        <v>25</v>
+      </c>
+      <c r="F31" s="60">
+        <f>COUNTIF(F3:F30, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+      <c r="G31" s="56">
+        <f>COUNTIF(G3:G30, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="60">
+        <f>COUNTIF(H3:H30, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="56">
+        <f>COUNTIF(I3:I30, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="57">
+        <f>COUNTIF(J3:J30, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="68"/>
+    </row>
+    <row r="32" spans="1:12" ht="17" thickBot="1">
+      <c r="A32" s="62"/>
+      <c r="B32" s="61">
+        <f t="shared" ref="B32:I32" si="3">B31/$A31</f>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="C32" s="61">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K24" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="16" customHeight="1">
-      <c r="A25" s="70" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="C25" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E25" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F25" s="72"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="76"/>
-      <c r="K25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="16" customHeight="1">
-      <c r="A26" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="C26" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="D26" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E26" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F26" s="72"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="76" t="str">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D32" s="61">
+        <f t="shared" ref="D32" si="4">D31/$A31</f>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="E32" s="63">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K26" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="16" customHeight="1">
-      <c r="A27" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="C27" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="D27" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E27" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F27" s="72"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="76" t="str">
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="F32" s="64">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="16" customHeight="1">
-      <c r="A28" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="C28" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="D28" s="72"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="76" t="str">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G32" s="63">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K28" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="16" customHeight="1">
-      <c r="A29" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="C29" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="D29" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E29" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="F29" s="72"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="76"/>
-      <c r="K29" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="16" customHeight="1">
-      <c r="A30" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="76" t="str">
+        <v>0</v>
+      </c>
+      <c r="H32" s="64">
         <f t="shared" si="3"/>
-        <v>Waiting for spec</v>
-      </c>
-      <c r="K30" s="76" t="str">
+        <v>0</v>
+      </c>
+      <c r="I32" s="63">
         <f t="shared" si="3"/>
-        <v>Waiting for spec</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="16" customHeight="1" thickBot="1">
-      <c r="A31" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="78"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="82"/>
-      <c r="J31" s="76" t="str">
-        <f t="shared" si="3"/>
-        <v>Waiting for spec</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="17" thickBot="1">
-      <c r="A32" s="58">
-        <f t="shared" ref="A32" si="4">COUNTIF(A3:A31, "&lt;&gt;")</f>
-        <v>29</v>
-      </c>
-      <c r="B32" s="59">
-        <f t="shared" ref="B32:H32" si="5">COUNTIF(B3:B31, "&lt;&gt;")</f>
-        <v>27</v>
-      </c>
-      <c r="C32" s="59">
-        <f t="shared" si="5"/>
-        <v>27</v>
-      </c>
-      <c r="D32" s="56">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="E32" s="60">
-        <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="F32" s="56">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G32" s="60">
-        <f t="shared" si="5"/>
+      <c r="J32" s="65">
+        <f t="shared" ref="J32" si="5">J31/$A31</f>
         <v>0</v>
       </c>
-      <c r="H32" s="56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="57">
-        <f t="shared" ref="I32" si="6">COUNTIF(I3:I31, "&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="68"/>
-    </row>
-    <row r="33" spans="1:10" ht="17" thickBot="1">
-      <c r="A33" s="62"/>
-      <c r="B33" s="61">
-        <f t="shared" ref="B33:H33" si="7">B32/$A32</f>
-        <v>0.93103448275862066</v>
-      </c>
-      <c r="C33" s="61">
-        <f t="shared" si="7"/>
-        <v>0.93103448275862066</v>
-      </c>
-      <c r="D33" s="63">
-        <f t="shared" si="7"/>
-        <v>0.7931034482758621</v>
-      </c>
-      <c r="E33" s="64">
-        <f t="shared" si="7"/>
-        <v>0.75862068965517238</v>
-      </c>
-      <c r="F33" s="63">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="64">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="63">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="65">
-        <f t="shared" ref="I33" si="8">I32/$A32</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="69"/>
+      <c r="K32" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:J18 A19:I31">
+  <conditionalFormatting sqref="A3:K30">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($B3="Yes", $C3="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19:J31 K30">
+  <conditionalFormatting sqref="L29">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($B19="Yes", $C19="")</formula>
+      <formula>AND($B29="Yes", $C29="")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tidied up profiles etc
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058A6E37-FC58-C649-B252-BAAC3696A5E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19F4EFB-5B87-9F4F-8BFC-455131295BE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="226">
   <si>
     <t>Welcome</t>
   </si>
@@ -765,7 +765,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1542,6 +1542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1554,7 +1555,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1914,7 +1914,7 @@
       <selection pane="bottomRight" activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="3" customWidth="1"/>
@@ -1925,7 +1925,7 @@
     <col min="13" max="30" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="31" customHeight="1">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>195</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="28" customFormat="1" ht="34">
+    <row r="8" spans="1:30" s="28" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>28</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="28" customFormat="1" ht="17">
+    <row r="9" spans="1:30" s="28" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
         <v>167</v>
       </c>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="X9"/>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>196</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>191</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>189</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>119</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:30" s="20" customFormat="1" ht="51">
+    <row r="39" spans="1:30" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>96</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>197</v>
       </c>
@@ -2912,7 +2912,7 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>198</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>200</v>
       </c>
@@ -3022,7 +3022,7 @@
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>198</v>
       </c>
@@ -3074,7 +3074,7 @@
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>201</v>
       </c>
@@ -3129,7 +3129,7 @@
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>198</v>
       </c>
@@ -3181,7 +3181,7 @@
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>202</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
     </row>
-    <row r="49" spans="2:30">
+    <row r="49" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B49" s="3" t="s">
         <v>198</v>
       </c>
@@ -3292,7 +3292,7 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
     </row>
-    <row r="50" spans="2:30">
+    <row r="50" spans="2:30" x14ac:dyDescent="0.2">
       <c r="G50" t="s">
         <v>205</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="2:30">
+    <row r="51" spans="2:30" x14ac:dyDescent="0.2">
       <c r="G51" t="s">
         <v>206</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="2:30">
+    <row r="52" spans="2:30" x14ac:dyDescent="0.2">
       <c r="G52" t="s">
         <v>207</v>
       </c>
@@ -3327,35 +3327,35 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" style="46" customWidth="1"/>
     <col min="11" max="11" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="50"/>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="83" t="s">
+      <c r="D1" s="83"/>
+      <c r="E1" s="84" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="83" t="s">
+      <c r="F1" s="85"/>
+      <c r="G1" s="84" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85" t="s">
+      <c r="H1" s="85"/>
+      <c r="I1" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="86"/>
+      <c r="J1" s="87"/>
       <c r="K1" s="66"/>
     </row>
-    <row r="2" spans="1:11" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="2" spans="1:11" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>211</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" customHeight="1">
+    <row r="3" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>212</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" customHeight="1">
+    <row r="4" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" customHeight="1">
+    <row r="5" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="70" t="s">
         <v>2</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" customHeight="1">
+    <row r="6" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="70" t="s">
         <v>3</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" customHeight="1">
+    <row r="7" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="70" t="s">
         <v>4</v>
       </c>
@@ -3512,7 +3512,9 @@
       <c r="C7" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D7" s="74"/>
+      <c r="D7" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E7" s="72" t="s">
         <v>221</v>
       </c>
@@ -3525,7 +3527,7 @@
       <c r="J7" s="75"/>
       <c r="K7" s="76"/>
     </row>
-    <row r="8" spans="1:11" ht="16" customHeight="1">
+    <row r="8" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="70" t="s">
         <v>5</v>
       </c>
@@ -3535,7 +3537,9 @@
       <c r="C8" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D8" s="74"/>
+      <c r="D8" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E8" s="72" t="s">
         <v>221</v>
       </c>
@@ -3551,7 +3555,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" customHeight="1">
+    <row r="9" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="70" t="s">
         <v>6</v>
       </c>
@@ -3561,7 +3565,9 @@
       <c r="C9" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D9" s="74"/>
+      <c r="D9" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E9" s="72" t="s">
         <v>221</v>
       </c>
@@ -3577,7 +3583,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" customHeight="1">
+    <row r="10" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="70" t="s">
         <v>7</v>
       </c>
@@ -3587,7 +3593,9 @@
       <c r="C10" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D10" s="74"/>
+      <c r="D10" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E10" s="72"/>
       <c r="F10" s="73" t="s">
         <v>221</v>
@@ -3601,7 +3609,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" customHeight="1">
+    <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="70" t="s">
         <v>8</v>
       </c>
@@ -3626,7 +3634,7 @@
       <c r="J11" s="75"/>
       <c r="K11" s="76"/>
     </row>
-    <row r="12" spans="1:11" ht="16" customHeight="1">
+    <row r="12" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="70" t="s">
         <v>10</v>
       </c>
@@ -3654,7 +3662,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" customHeight="1">
+    <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="70" t="s">
         <v>11</v>
       </c>
@@ -3664,7 +3672,9 @@
       <c r="C13" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D13" s="74"/>
+      <c r="D13" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E13" s="72" t="s">
         <v>221</v>
       </c>
@@ -3680,7 +3690,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" customHeight="1">
+    <row r="14" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="70" t="s">
         <v>213</v>
       </c>
@@ -3705,7 +3715,7 @@
       <c r="J14" s="75"/>
       <c r="K14" s="76"/>
     </row>
-    <row r="15" spans="1:11" ht="16" customHeight="1">
+    <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="70" t="s">
         <v>12</v>
       </c>
@@ -3715,7 +3725,9 @@
       <c r="C15" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D15" s="74"/>
+      <c r="D15" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E15" s="72" t="s">
         <v>221</v>
       </c>
@@ -3728,7 +3740,7 @@
       <c r="J15" s="75"/>
       <c r="K15" s="76"/>
     </row>
-    <row r="16" spans="1:11" ht="16" customHeight="1">
+    <row r="16" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="70" t="s">
         <v>214</v>
       </c>
@@ -3756,7 +3768,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16" customHeight="1">
+    <row r="17" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="70" t="s">
         <v>122</v>
       </c>
@@ -3784,7 +3796,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="17">
+    <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="70" t="s">
         <v>215</v>
       </c>
@@ -3809,7 +3821,7 @@
       <c r="J18" s="75"/>
       <c r="K18" s="76"/>
     </row>
-    <row r="19" spans="1:12" ht="16" customHeight="1">
+    <row r="19" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="70" t="s">
         <v>13</v>
       </c>
@@ -3837,7 +3849,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="16" customHeight="1">
+    <row r="20" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="70" t="s">
         <v>154</v>
       </c>
@@ -3847,7 +3859,9 @@
       <c r="C20" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D20" s="74"/>
+      <c r="D20" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E20" s="72" t="s">
         <v>221</v>
       </c>
@@ -3863,7 +3877,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="16" customHeight="1">
+    <row r="21" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="70" t="s">
         <v>155</v>
       </c>
@@ -3873,7 +3887,9 @@
       <c r="C21" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="74"/>
+      <c r="D21" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E21" s="72" t="s">
         <v>221</v>
       </c>
@@ -3889,7 +3905,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="16" customHeight="1">
+    <row r="22" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="70" t="s">
         <v>14</v>
       </c>
@@ -3899,7 +3915,9 @@
       <c r="C22" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D22" s="74"/>
+      <c r="D22" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E22" s="72" t="s">
         <v>221</v>
       </c>
@@ -3915,7 +3933,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16" customHeight="1">
+    <row r="23" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="70" t="s">
         <v>15</v>
       </c>
@@ -3938,7 +3956,7 @@
       <c r="J23" s="75"/>
       <c r="K23" s="76"/>
     </row>
-    <row r="24" spans="1:12" ht="16" customHeight="1">
+    <row r="24" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="70" t="s">
         <v>17</v>
       </c>
@@ -3948,7 +3966,9 @@
       <c r="C24" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="74"/>
+      <c r="D24" s="74" t="s">
+        <v>221</v>
+      </c>
       <c r="E24" s="72" t="s">
         <v>221</v>
       </c>
@@ -3961,7 +3981,7 @@
       <c r="J24" s="75"/>
       <c r="K24" s="76"/>
     </row>
-    <row r="25" spans="1:12" ht="16" customHeight="1">
+    <row r="25" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="70" t="s">
         <v>18</v>
       </c>
@@ -3989,7 +4009,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16" customHeight="1">
+    <row r="26" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="70" t="s">
         <v>19</v>
       </c>
@@ -4017,7 +4037,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="16" customHeight="1">
+    <row r="27" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="70" t="s">
         <v>20</v>
       </c>
@@ -4045,7 +4065,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16" customHeight="1">
+    <row r="28" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="70" t="s">
         <v>21</v>
       </c>
@@ -4070,7 +4090,7 @@
       <c r="J28" s="75"/>
       <c r="K28" s="76"/>
     </row>
-    <row r="29" spans="1:12" ht="16" customHeight="1">
+    <row r="29" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="70" t="s">
         <v>22</v>
       </c>
@@ -4089,7 +4109,7 @@
       </c>
       <c r="L29" s="76"/>
     </row>
-    <row r="30" spans="1:12" ht="16" customHeight="1" thickBot="1">
+    <row r="30" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
         <v>23</v>
       </c>
@@ -4107,85 +4127,85 @@
         <v>Waiting for spec</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="17" thickBot="1">
+    <row r="31" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="58">
-        <f>COUNTIF(A3:A30, "&lt;&gt;")</f>
+        <f t="shared" ref="A31:J31" si="3">COUNTIF(A3:A30, "&lt;&gt;")</f>
         <v>28</v>
       </c>
       <c r="B31" s="59">
-        <f>COUNTIF(B3:B30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="C31" s="59">
-        <f>COUNTIF(C3:C30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="D31" s="59">
-        <f>COUNTIF(D3:D30, "&lt;&gt;")</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
       <c r="E31" s="56">
-        <f>COUNTIF(E3:E30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="F31" s="60">
-        <f>COUNTIF(F3:F30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="G31" s="56">
-        <f>COUNTIF(G3:G30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H31" s="60">
-        <f>COUNTIF(H3:H30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I31" s="56">
-        <f>COUNTIF(I3:I30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J31" s="57">
-        <f>COUNTIF(J3:J30, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K31" s="68"/>
     </row>
-    <row r="32" spans="1:12" ht="17" thickBot="1">
+    <row r="32" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="62"/>
       <c r="B32" s="61">
-        <f t="shared" ref="B32:I32" si="3">B31/$A31</f>
+        <f t="shared" ref="B32:I32" si="4">B31/$A31</f>
         <v>0.9285714285714286</v>
       </c>
       <c r="C32" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9285714285714286</v>
       </c>
       <c r="D32" s="61">
-        <f t="shared" ref="D32" si="4">D31/$A31</f>
-        <v>0.5357142857142857</v>
+        <f t="shared" ref="D32" si="5">D31/$A31</f>
+        <v>0.8928571428571429</v>
       </c>
       <c r="E32" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8928571428571429</v>
       </c>
       <c r="F32" s="64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9285714285714286</v>
       </c>
       <c r="G32" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H32" s="64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I32" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J32" s="65">
-        <f t="shared" ref="J32" si="5">J31/$A31</f>
+        <f t="shared" ref="J32" si="6">J31/$A31</f>
         <v>0</v>
       </c>
       <c r="K32" s="69"/>

</xml_diff>

<commit_message>
Latest version of help
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19F4EFB-5B87-9F4F-8BFC-455131295BE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A839CB23-936A-964D-8EC2-5AEE759CF344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="227">
   <si>
     <t>Welcome</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Help</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1524,25 +1527,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1553,6 +1541,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1560,17 +1551,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3324,38 +3305,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD168BF6-7604-814B-8525-59664C788955}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" style="46" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="50"/>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84" t="s">
+      <c r="D1" s="77"/>
+      <c r="E1" s="79" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="84" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="85"/>
-      <c r="I1" s="86" t="s">
+      <c r="H1" s="80"/>
+      <c r="I1" s="81" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="87"/>
-      <c r="K1" s="66"/>
-    </row>
-    <row r="2" spans="1:11" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="82"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="66"/>
+    </row>
+    <row r="2" spans="1:12" s="47" customFormat="1" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>211</v>
       </c>
@@ -3386,11 +3368,14 @@
       <c r="J2" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="49" t="s">
+        <v>226</v>
+      </c>
+      <c r="L2" s="67" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>212</v>
       </c>
@@ -3413,12 +3398,15 @@
       <c r="H3" s="73"/>
       <c r="I3" s="74"/>
       <c r="J3" s="75"/>
-      <c r="K3" s="76" t="str">
-        <f t="shared" ref="K3:K6" si="0">IF(B3="","Waiting for spec","")</f>
+      <c r="K3" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L3" s="76" t="str">
+        <f t="shared" ref="L3:L6" si="0">IF(B3="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
@@ -3441,12 +3429,13 @@
       <c r="H4" s="73"/>
       <c r="I4" s="74"/>
       <c r="J4" s="75"/>
-      <c r="K4" s="76" t="str">
+      <c r="K4" s="75"/>
+      <c r="L4" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="70" t="s">
         <v>2</v>
       </c>
@@ -3469,12 +3458,15 @@
       <c r="H5" s="73"/>
       <c r="I5" s="74"/>
       <c r="J5" s="75"/>
-      <c r="K5" s="76" t="str">
+      <c r="K5" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="L5" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="70" t="s">
         <v>3</v>
       </c>
@@ -3497,12 +3489,15 @@
       <c r="H6" s="73"/>
       <c r="I6" s="74"/>
       <c r="J6" s="75"/>
-      <c r="K6" s="76" t="str">
+      <c r="K6" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="L6" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="70" t="s">
         <v>4</v>
       </c>
@@ -3525,9 +3520,10 @@
       <c r="H7" s="73"/>
       <c r="I7" s="74"/>
       <c r="J7" s="75"/>
-      <c r="K7" s="76"/>
-    </row>
-    <row r="8" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="75"/>
+      <c r="L7" s="76"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="70" t="s">
         <v>5</v>
       </c>
@@ -3550,12 +3546,13 @@
       <c r="H8" s="73"/>
       <c r="I8" s="74"/>
       <c r="J8" s="75"/>
-      <c r="K8" s="76" t="str">
-        <f t="shared" ref="K8:K9" si="1">IF(B8="","Waiting for spec","")</f>
+      <c r="K8" s="75"/>
+      <c r="L8" s="76" t="str">
+        <f t="shared" ref="L8:L9" si="1">IF(B8="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="70" t="s">
         <v>6</v>
       </c>
@@ -3578,12 +3575,13 @@
       <c r="H9" s="73"/>
       <c r="I9" s="74"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="76" t="str">
+      <c r="K9" s="75"/>
+      <c r="L9" s="76" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="70" t="s">
         <v>7</v>
       </c>
@@ -3604,12 +3602,13 @@
       <c r="H10" s="73"/>
       <c r="I10" s="74"/>
       <c r="J10" s="75"/>
-      <c r="K10" s="76" t="str">
-        <f t="shared" ref="K10:K17" si="2">IF(B10="","Waiting for spec","")</f>
+      <c r="K10" s="75"/>
+      <c r="L10" s="76" t="str">
+        <f t="shared" ref="L10:L17" si="2">IF(B10="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="70" t="s">
         <v>8</v>
       </c>
@@ -3632,9 +3631,10 @@
       <c r="H11" s="73"/>
       <c r="I11" s="74"/>
       <c r="J11" s="75"/>
-      <c r="K11" s="76"/>
-    </row>
-    <row r="12" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="75"/>
+      <c r="L11" s="76"/>
+    </row>
+    <row r="12" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="70" t="s">
         <v>10</v>
       </c>
@@ -3657,12 +3657,15 @@
       <c r="H12" s="73"/>
       <c r="I12" s="74"/>
       <c r="J12" s="75"/>
-      <c r="K12" s="76" t="str">
+      <c r="K12" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="L12" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="70" t="s">
         <v>11</v>
       </c>
@@ -3685,12 +3688,13 @@
       <c r="H13" s="73"/>
       <c r="I13" s="74"/>
       <c r="J13" s="75"/>
-      <c r="K13" s="76" t="str">
+      <c r="K13" s="75"/>
+      <c r="L13" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="70" t="s">
         <v>213</v>
       </c>
@@ -3713,9 +3717,12 @@
       <c r="H14" s="73"/>
       <c r="I14" s="74"/>
       <c r="J14" s="75"/>
-      <c r="K14" s="76"/>
-    </row>
-    <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L14" s="76"/>
+    </row>
+    <row r="15" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="70" t="s">
         <v>12</v>
       </c>
@@ -3738,9 +3745,10 @@
       <c r="H15" s="73"/>
       <c r="I15" s="74"/>
       <c r="J15" s="75"/>
-      <c r="K15" s="76"/>
-    </row>
-    <row r="16" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="75"/>
+      <c r="L15" s="76"/>
+    </row>
+    <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="70" t="s">
         <v>214</v>
       </c>
@@ -3763,7 +3771,8 @@
       <c r="H16" s="73"/>
       <c r="I16" s="74"/>
       <c r="J16" s="75"/>
-      <c r="K16" s="76" t="str">
+      <c r="K16" s="75"/>
+      <c r="L16" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3791,7 +3800,8 @@
       <c r="H17" s="73"/>
       <c r="I17" s="74"/>
       <c r="J17" s="75"/>
-      <c r="K17" s="76" t="str">
+      <c r="K17" s="75"/>
+      <c r="L17" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3819,7 +3829,8 @@
       <c r="H18" s="73"/>
       <c r="I18" s="74"/>
       <c r="J18" s="75"/>
-      <c r="K18" s="76"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="76"/>
     </row>
     <row r="19" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="70" t="s">
@@ -3844,7 +3855,8 @@
       <c r="H19" s="73"/>
       <c r="I19" s="74"/>
       <c r="J19" s="75"/>
-      <c r="K19" s="76" t="str">
+      <c r="K19" s="75"/>
+      <c r="L19" s="76" t="str">
         <f>IF(B19="","Waiting for spec","")</f>
         <v/>
       </c>
@@ -3872,7 +3884,8 @@
       <c r="H20" s="73"/>
       <c r="I20" s="74"/>
       <c r="J20" s="75"/>
-      <c r="K20" s="76" t="str">
+      <c r="K20" s="75"/>
+      <c r="L20" s="76" t="str">
         <f>IF(B20="","Waiting for spec","")</f>
         <v/>
       </c>
@@ -3900,7 +3913,8 @@
       <c r="H21" s="73"/>
       <c r="I21" s="74"/>
       <c r="J21" s="75"/>
-      <c r="K21" s="76" t="str">
+      <c r="K21" s="75"/>
+      <c r="L21" s="76" t="str">
         <f>IF(B21="","Waiting for spec","")</f>
         <v/>
       </c>
@@ -3928,7 +3942,8 @@
       <c r="H22" s="73"/>
       <c r="I22" s="74"/>
       <c r="J22" s="75"/>
-      <c r="K22" s="76" t="str">
+      <c r="K22" s="75"/>
+      <c r="L22" s="76" t="str">
         <f>IF(B22="","Waiting for spec","")</f>
         <v/>
       </c>
@@ -3954,7 +3969,8 @@
       <c r="H23" s="73"/>
       <c r="I23" s="74"/>
       <c r="J23" s="75"/>
-      <c r="K23" s="76"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="76"/>
     </row>
     <row r="24" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="70" t="s">
@@ -3979,7 +3995,10 @@
       <c r="H24" s="73"/>
       <c r="I24" s="74"/>
       <c r="J24" s="75"/>
-      <c r="K24" s="76"/>
+      <c r="K24" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L24" s="76"/>
     </row>
     <row r="25" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="70" t="s">
@@ -4004,7 +4023,10 @@
       <c r="H25" s="73"/>
       <c r="I25" s="74"/>
       <c r="J25" s="75"/>
-      <c r="K25" s="76" t="str">
+      <c r="K25" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="L25" s="76" t="str">
         <f>IF(B25="","Waiting for spec","")</f>
         <v/>
       </c>
@@ -4032,7 +4054,10 @@
       <c r="H26" s="73"/>
       <c r="I26" s="74"/>
       <c r="J26" s="75"/>
-      <c r="K26" s="76" t="str">
+      <c r="K26" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L26" s="76" t="str">
         <f>IF(B26="","Waiting for spec","")</f>
         <v/>
       </c>
@@ -4060,12 +4085,15 @@
       <c r="H27" s="73"/>
       <c r="I27" s="74"/>
       <c r="J27" s="75"/>
-      <c r="K27" s="76" t="str">
+      <c r="K27" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L27" s="76" t="str">
         <f>IF(B27="","Waiting for spec","")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="70" t="s">
         <v>21</v>
       </c>
@@ -4088,127 +4116,93 @@
       <c r="H28" s="73"/>
       <c r="I28" s="74"/>
       <c r="J28" s="75"/>
-      <c r="K28" s="76"/>
-    </row>
-    <row r="29" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="76" t="str">
-        <f>IF(B29="","Waiting for spec","")</f>
-        <v>Waiting for spec</v>
-      </c>
-      <c r="L29" s="76"/>
-    </row>
-    <row r="30" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="78"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="76" t="str">
-        <f>IF(B30="","Waiting for spec","")</f>
-        <v>Waiting for spec</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="58">
-        <f t="shared" ref="A31:J31" si="3">COUNTIF(A3:A30, "&lt;&gt;")</f>
-        <v>28</v>
-      </c>
-      <c r="B31" s="59">
+      <c r="K28" s="75"/>
+      <c r="L28" s="76"/>
+    </row>
+    <row r="29" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58">
+        <f>COUNTIF(A3:A28, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+      <c r="B29" s="59">
+        <f>COUNTIF(B3:B28, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+      <c r="C29" s="59">
+        <f>COUNTIF(C3:C28, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+      <c r="D29" s="59">
+        <f>COUNTIF(D3:D28, "&lt;&gt;")</f>
+        <v>25</v>
+      </c>
+      <c r="E29" s="56">
+        <f>COUNTIF(E3:E28, "&lt;&gt;")</f>
+        <v>25</v>
+      </c>
+      <c r="F29" s="60">
+        <f>COUNTIF(F3:F28, "&lt;&gt;")</f>
+        <v>26</v>
+      </c>
+      <c r="G29" s="56">
+        <f>COUNTIF(G3:G28, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="60">
+        <f>COUNTIF(H3:H28, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="56">
+        <f>COUNTIF(I3:I28, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="57">
+        <f>COUNTIF(J3:J28, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="57"/>
+      <c r="L29" s="68"/>
+    </row>
+    <row r="30" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="62"/>
+      <c r="B30" s="61">
+        <f t="shared" ref="B30:I30" si="3">B29/$A29</f>
+        <v>1</v>
+      </c>
+      <c r="C30" s="61">
         <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="C31" s="59">
+        <v>1</v>
+      </c>
+      <c r="D30" s="61">
+        <f t="shared" ref="D30" si="4">D29/$A29</f>
+        <v>0.96153846153846156</v>
+      </c>
+      <c r="E30" s="63">
         <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="D31" s="59">
+        <v>0.96153846153846156</v>
+      </c>
+      <c r="F30" s="64">
         <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="E31" s="56">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="F31" s="60">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="G31" s="56">
+        <v>1</v>
+      </c>
+      <c r="G30" s="63">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" s="60">
+      <c r="H30" s="64">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I31" s="56">
+      <c r="I30" s="63">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J31" s="57">
-        <f t="shared" si="3"/>
+      <c r="J30" s="65">
+        <f t="shared" ref="J30" si="5">J29/$A29</f>
         <v>0</v>
       </c>
-      <c r="K31" s="68"/>
-    </row>
-    <row r="32" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="61">
-        <f t="shared" ref="B32:I32" si="4">B31/$A31</f>
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="C32" s="61">
-        <f t="shared" si="4"/>
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="D32" s="61">
-        <f t="shared" ref="D32" si="5">D31/$A31</f>
-        <v>0.8928571428571429</v>
-      </c>
-      <c r="E32" s="63">
-        <f t="shared" si="4"/>
-        <v>0.8928571428571429</v>
-      </c>
-      <c r="F32" s="64">
-        <f t="shared" si="4"/>
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="G32" s="63">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="64">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="63">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="65">
-        <f t="shared" ref="J32" si="6">J31/$A31</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="69"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4216,14 +4210,9 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:K30">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A3:L28">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND($B3="Yes", $C3="")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L29">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($B29="Yes", $C29="")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Yet another iteration of help this time including location
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A839CB23-936A-964D-8EC2-5AEE759CF344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E34C4A8-FBA4-1F4E-88A8-BAD089426097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="227">
   <si>
     <t>Welcome</t>
   </si>
@@ -1309,7 +1309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1541,9 +1541,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3308,7 +3305,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3631,7 +3628,9 @@
       <c r="H11" s="73"/>
       <c r="I11" s="74"/>
       <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
+      <c r="K11" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L11" s="76"/>
     </row>
     <row r="12" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4121,87 +4120,93 @@
     </row>
     <row r="29" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="58">
-        <f>COUNTIF(A3:A28, "&lt;&gt;")</f>
+        <f t="shared" ref="A29:K29" si="3">COUNTIF(A3:A28, "&lt;&gt;")</f>
         <v>26</v>
       </c>
       <c r="B29" s="59">
-        <f>COUNTIF(B3:B28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="C29" s="59">
-        <f>COUNTIF(C3:C28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="D29" s="59">
-        <f>COUNTIF(D3:D28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="E29" s="56">
-        <f>COUNTIF(E3:E28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="F29" s="60">
-        <f>COUNTIF(F3:F28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="G29" s="56">
-        <f>COUNTIF(G3:G28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H29" s="60">
-        <f>COUNTIF(H3:H28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I29" s="56">
-        <f>COUNTIF(I3:I28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J29" s="57">
-        <f>COUNTIF(J3:J28, "&lt;&gt;")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K29" s="57"/>
+      <c r="K29" s="59">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
       <c r="L29" s="68"/>
     </row>
     <row r="30" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="62"/>
       <c r="B30" s="61">
-        <f t="shared" ref="B30:I30" si="3">B29/$A29</f>
+        <f t="shared" ref="B30:I30" si="4">B29/$A29</f>
         <v>1</v>
       </c>
       <c r="C30" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D30" s="61">
-        <f t="shared" ref="D30" si="4">D29/$A29</f>
+        <f t="shared" ref="D30" si="5">D29/$A29</f>
         <v>0.96153846153846156</v>
       </c>
       <c r="E30" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.96153846153846156</v>
       </c>
       <c r="F30" s="64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G30" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H30" s="64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I30" s="63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J30" s="65">
-        <f t="shared" ref="J30" si="5">J29/$A29</f>
+        <f t="shared" ref="J30:K30" si="6">J29/$A29</f>
         <v>0</v>
       </c>
-      <c r="K30" s="83"/>
+      <c r="K30" s="61">
+        <f t="shared" si="6"/>
+        <v>0.38461538461538464</v>
+      </c>
       <c r="L30" s="69"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement help fo game summary and game detail and also improve sort sequence of menu/banner controls
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E34C4A8-FBA4-1F4E-88A8-BAD089426097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA2A93C-420D-7949-8BEC-BF0F7A190059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="227">
   <si>
     <t>Welcome</t>
   </si>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3517,7 +3517,9 @@
       <c r="H7" s="73"/>
       <c r="I7" s="74"/>
       <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="K7" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L7" s="76"/>
     </row>
     <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3543,7 +3545,9 @@
       <c r="H8" s="73"/>
       <c r="I8" s="74"/>
       <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
+      <c r="K8" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L8" s="76" t="str">
         <f t="shared" ref="L8:L9" si="1">IF(B8="","Waiting for spec","")</f>
         <v/>
@@ -3572,7 +3576,9 @@
       <c r="H9" s="73"/>
       <c r="I9" s="74"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
+      <c r="K9" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L9" s="76" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3599,7 +3605,9 @@
       <c r="H10" s="73"/>
       <c r="I10" s="74"/>
       <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="K10" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L10" s="76" t="str">
         <f t="shared" ref="L10:L17" si="2">IF(B10="","Waiting for spec","")</f>
         <v/>
@@ -4161,7 +4169,7 @@
       </c>
       <c r="K29" s="59">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L29" s="68"/>
     </row>
@@ -4205,7 +4213,7 @@
       </c>
       <c r="K30" s="61">
         <f t="shared" si="6"/>
-        <v>0.38461538461538464</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="L30" s="69"/>
     </row>

</xml_diff>

<commit_message>
Added support for dashboard views to help
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA2A93C-420D-7949-8BEC-BF0F7A190059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663AACE1-E7C4-CF40-B426-3D592F64ADA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="227">
   <si>
     <t>Welcome</t>
   </si>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3862,7 +3862,9 @@
       <c r="H19" s="73"/>
       <c r="I19" s="74"/>
       <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
+      <c r="K19" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L19" s="76" t="str">
         <f>IF(B19="","Waiting for spec","")</f>
         <v/>
@@ -3949,7 +3951,9 @@
       <c r="H22" s="73"/>
       <c r="I22" s="74"/>
       <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
+      <c r="K22" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L22" s="76" t="str">
         <f>IF(B22="","Waiting for spec","")</f>
         <v/>
@@ -4169,7 +4173,7 @@
       </c>
       <c r="K29" s="59">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L29" s="68"/>
     </row>
@@ -4213,7 +4217,7 @@
       </c>
       <c r="K30" s="61">
         <f t="shared" si="6"/>
-        <v>0.53846153846153844</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="L30" s="69"/>
     </row>

</xml_diff>

<commit_message>
Statistics and History help
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663AACE1-E7C4-CF40-B426-3D592F64ADA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB31EFF-3788-3842-A14C-AE8414748633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="227">
   <si>
     <t>Welcome</t>
   </si>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3836,7 +3836,9 @@
       <c r="H18" s="73"/>
       <c r="I18" s="74"/>
       <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
+      <c r="K18" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L18" s="76"/>
     </row>
     <row r="19" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4173,7 +4175,7 @@
       </c>
       <c r="K29" s="59">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L29" s="68"/>
     </row>
@@ -4217,7 +4219,7 @@
       </c>
       <c r="K30" s="61">
         <f t="shared" si="6"/>
-        <v>0.61538461538461542</v>
+        <v>0.65384615384615385</v>
       </c>
       <c r="L30" s="69"/>
     </row>

</xml_diff>

<commit_message>
Version where popups work for confirm views (not others)
</commit_message>
<xml_diff>
--- a/Contract Whist Scorecard/Colors.xlsx
+++ b/Contract Whist Scorecard/Colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcshearer/Documents/Xcode projects/Contract Whist Scorecard/Contract Whist Scorecard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9703C9D0-0FA6-C043-BF92-3231B6908B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D56F6-8C13-E646-99BD-A7438318C58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
+    <workbookView xWindow="4060" yWindow="1040" windowWidth="23580" windowHeight="17440" activeTab="1" xr2:uid="{A195F82B-EE89-444A-A2DE-9F3BE0B609E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="227">
   <si>
     <t>Welcome</t>
   </si>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3426,7 +3426,9 @@
       <c r="H4" s="73"/>
       <c r="I4" s="74"/>
       <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
+      <c r="K4" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L4" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3695,7 +3697,9 @@
       <c r="H13" s="73"/>
       <c r="I13" s="74"/>
       <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
+      <c r="K13" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L13" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3752,7 +3756,9 @@
       <c r="H15" s="73"/>
       <c r="I15" s="74"/>
       <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
+      <c r="K15" s="75" t="s">
+        <v>225</v>
+      </c>
       <c r="L15" s="76"/>
     </row>
     <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3778,7 +3784,9 @@
       <c r="H16" s="73"/>
       <c r="I16" s="74"/>
       <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
+      <c r="K16" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L16" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3807,7 +3815,9 @@
       <c r="H17" s="73"/>
       <c r="I17" s="74"/>
       <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
+      <c r="K17" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L17" s="76" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3986,7 +3996,9 @@
       <c r="H23" s="73"/>
       <c r="I23" s="74"/>
       <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
+      <c r="K23" s="75" t="s">
+        <v>221</v>
+      </c>
       <c r="L23" s="76"/>
     </row>
     <row r="24" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4179,7 +4191,7 @@
       </c>
       <c r="K29" s="59">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="L29" s="68"/>
     </row>
@@ -4223,7 +4235,7 @@
       </c>
       <c r="K30" s="61">
         <f t="shared" si="6"/>
-        <v>0.73076923076923073</v>
+        <v>0.96153846153846156</v>
       </c>
       <c r="L30" s="69"/>
     </row>

</xml_diff>